<commit_message>
Konsolidierung; Gliederung und Jankowiz Artikel
</commit_message>
<xml_diff>
--- a/Review.xlsx
+++ b/Review.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sven\Documents\GitHub\AR-Education\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="-435" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="231">
   <si>
     <t>Title</t>
   </si>
@@ -627,12 +632,161 @@
 mode affected the subject’s attitude, and it resulted in behavior
 change.</t>
   </si>
+  <si>
+    <t>"lead to an increased ability to retain long term memories"</t>
+  </si>
+  <si>
+    <t>improved memory</t>
+  </si>
+  <si>
+    <t>This appears to indicate that certain modes of
+presentation (i.e., AR and IAR) produced better learning and retention of information since the amount of
+information loss between the IR test and the LTR test
+was minimal and not statistically significant.</t>
+  </si>
+  <si>
+    <t>"had higher motivation"</t>
+  </si>
+  <si>
+    <t>"had higher [...] and degree of concentration"</t>
+  </si>
+  <si>
+    <t>The results support the hypothesis, and suggest that Augmented Reality has some potential to be effective in aiding the learning of 3D concepts.</t>
+  </si>
+  <si>
+    <t>development of spatial abilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">his supports the notion that AR books can help in learning complex three dimensional concepts </t>
+  </si>
+  <si>
+    <t>developmentof spatial abilities</t>
+  </si>
+  <si>
+    <t>The interactivity afforded by AR books provides great potential for learning and an advantage over traditional books or other learning media. Tangible interaction using tools such as the magnet paddle and augmented nail with labeled poles allow for a learning experience that combines real world objects with virtual content. Together this can contribute to a deeper understanding. Interactions in AR engage learners with the content, and allow for knowledge to be acquired through their own manipulation of content (Dünser, 2008), as supported by constructivist learning theory (Tobias &amp; Duffy, 2009 ).</t>
+  </si>
+  <si>
+    <t>Participants using the AR books appeared much more
+eager at the beginning of each session compared with the
+NAR group.</t>
+  </si>
+  <si>
+    <t>increased motivation</t>
+  </si>
+  <si>
+    <t>Contibution to deeper understanding through interaction with a combination of real world objects and virtual content</t>
+  </si>
+  <si>
+    <t>deeper learning through the combination of real world objects and virtual content</t>
+  </si>
+  <si>
+    <t>The AR-guided group had better learning effectiveness (as evidenced by their posttest scores), and it was found that most visitors believed the AR guide made it easier to digest information than the audio guide due to the extra visual commentary that is provided. This mode not only offers an audio commentary, but also displays visual information dominated by text and images.</t>
+  </si>
+  <si>
+    <t>It facilitates the development of art appreciation by imprinting the knowledge of paintings on visitors’ memories, supporting the coupling between the visitors, the guide system, and the artwork (Klopfer &amp; Squire, 2008) by using AR technology, and helping visitorskeep their memories of the artwork vivid.</t>
+  </si>
+  <si>
+    <t>Overall the visitors using the mobile AR-guide system during painting appreciation activities felt that it was an interesting, innovative, creative, and entertaining guide device;</t>
+  </si>
+  <si>
+    <t>The learning performance of the AR-guided group was thus superior to
+that of the other two groups.</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Post-hoc comparisons showed that the time spent focusing on paintings was significantly
+longer for both the AR-guided (mean ¼ 17.3278 min) and audio-guided (mean ¼ 16.114 min) groups than for the nonguided group
+(mean ¼ 4.76 min). The focusing time did not differ significantly between the AR-guided and audio-guided groups.</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Analysis of the flow experience revealed that the visitors in the AR-guided group were clearly more ready to enter the state of flow with
+respect to the antecedents of flow, and were more proactive in appreciating the artwork than were those in the other two groups. During the
+activity, those in the audio-guided and AR-guided groups expressed the flow states obviously.</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>improved creativity</t>
+  </si>
+  <si>
+    <t>improved attention</t>
+  </si>
+  <si>
+    <t>In addition, the participants appeared to be highly interested in using the system to observe lunar phase, with the mean of Q8 being 4.10. Participants agreed that the system is helpful to them in enhancing their motivation</t>
+  </si>
+  <si>
+    <t>The results of our research support this characterization, as the teachers reported high levels of student engagement with the technology, and also with science. Students’ engagement with the technology was also evident in their responses to the opinion post-survey, in which technology-rich activities were rated higher than those without technology.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We observed gains in a number of affective items and saw particular gains in student self-efficacy and their understanding of what scientists do. </t>
+  </si>
+  <si>
+    <t>improved self-efficacy</t>
+  </si>
+  <si>
+    <t>Using augmented reality on the field trip allowed teachers to use pedagogical approaches that may otherwise be difficult in an outdoor learning environment. The technology supported independence, as students navigated to the AR trigger locations to explore and learn at their own pace. This freed the teacher to act as facilitator, an affordance of AR that has been hypothesized by other researchers (Roschelle &amp; Pea, 2002). The teachers also highlighted this as one of the greatest benefits to teaching with the mobile devices. The program director shared her thoughts saying Such feedback suggests that AR can provide a powerful pedagogical tool that supports student-centered learning.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">these technologies provide ways of individualizing instruction in a group setting, fostering increased motivation and learning </t>
+  </si>
+  <si>
+    <t>We witnessed significant learning gains on the content survey (T(70,1) ¼  8.53, based on paired t-test). Students’ scores went up by an
+average of 19% from the pre to post survey (Mean_pre ¼ 4.3   1.8, Mean_post ¼ 5.9   1.9, based on 9 total points). The effect size associated
+with these gains was substantial (1.0), indicating that student gains were equivalent to one standard deviation around the mean of the data.</t>
+  </si>
+  <si>
+    <t>Prior to the field trip, two of the teachers had expressed concern that the smartphones might be too engaging; leading students to ignore
+the real environment in favor of the media and capabilities provided by the smartphones. Post-field trip comments indicated the contrary
+was true – teachers noted that the smartphones promoted interaction with the pond and classmates.</t>
+  </si>
+  <si>
+    <t>Teachers commented that the smartphones helped to structure students’ movement through space and guided their interaction with the
+pond and with classmates. The students were able to work independently, at their own pace, with the teacher acting as a facilitator. Teachers
+reported that the activities were more student-driven and less teacher-directed.</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Another feature of the activity was the opportunity for collaborative communication and problem-solving among students that arose
+from the augmented reality experience.</t>
+  </si>
+  <si>
+    <t>Written feedback from the teachers indicated that AR was particularly useful in engaging students.</t>
+  </si>
+  <si>
+    <t>9-11</t>
+  </si>
+  <si>
+    <t>student centered learning</t>
+  </si>
+  <si>
+    <t>independence</t>
+  </si>
+  <si>
+    <t>individualization</t>
+  </si>
+  <si>
+    <t>improved learning curve</t>
+  </si>
+  <si>
+    <t>improved collaborative learning</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -674,6 +828,11 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="TimesNewRoman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="TimesNewRomanPSMT"/>
     </font>
   </fonts>
   <fills count="5">
@@ -743,7 +902,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -759,27 +918,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="21">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1060,7 +1229,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1068,21 +1237,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K72"/>
+  <dimension ref="A1:K92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="16.1640625" customWidth="1"/>
-    <col min="8" max="8" width="57" customWidth="1"/>
-    <col min="10" max="10" width="22.83203125" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="57" style="8" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="14"/>
+    <col min="10" max="10" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1107,10 +1278,10 @@
       <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="13" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -1140,7 +1311,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="70">
+    <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1162,16 +1333,16 @@
       <c r="G3" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="15" t="s">
         <v>151</v>
       </c>
       <c r="J3" t="s">
         <v>138</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="9" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1185,7 +1356,7 @@
       <c r="H4" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="16">
         <v>253</v>
       </c>
       <c r="J4" t="s">
@@ -1205,7 +1376,7 @@
       <c r="H5" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="16">
         <v>254</v>
       </c>
       <c r="J5" s="7" t="s">
@@ -1237,7 +1408,7 @@
       <c r="H6" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="14">
         <v>525</v>
       </c>
       <c r="J6" s="2" t="s">
@@ -1307,7 +1478,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="28">
+    <row r="10" spans="1:11">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1329,10 +1500,10 @@
       <c r="G10" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="15" t="s">
         <v>158</v>
       </c>
       <c r="J10" s="2" t="s">
@@ -1347,17 +1518,17 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="15" t="s">
         <v>158</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="28">
+    <row r="12" spans="1:11">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1365,10 +1536,10 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="15" t="s">
         <v>158</v>
       </c>
       <c r="J12" s="2" t="s">
@@ -1386,7 +1557,7 @@
       <c r="H13" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="14">
         <v>894</v>
       </c>
       <c r="J13" s="2" t="s">
@@ -1401,17 +1572,17 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="14">
         <v>894</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="112">
+    <row r="15" spans="1:11">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
@@ -1433,17 +1604,17 @@
       <c r="G15" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="15" t="s">
         <v>158</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="28">
+    <row r="16" spans="1:11">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1451,17 +1622,17 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="15" t="s">
         <v>169</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="56">
+    <row r="17" spans="1:11">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1469,10 +1640,10 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="14">
         <v>5</v>
       </c>
       <c r="J17" s="2" t="s">
@@ -1504,24 +1675,24 @@
       <c r="H18" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="14">
         <v>56</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="70">
+    <row r="19" spans="1:11">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="14">
         <v>5</v>
       </c>
       <c r="J19" s="2" t="s">
@@ -1573,14 +1744,14 @@
       <c r="H21" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="I21" s="9" t="s">
+      <c r="I21" s="15" t="s">
         <v>178</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="42">
+    <row r="22" spans="1:11">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1602,61 +1773,61 @@
       <c r="G22" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="14">
         <v>8</v>
       </c>
       <c r="J22" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="84">
+    <row r="23" spans="1:11">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="H23" s="11" t="s">
+      <c r="H23" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="14">
         <v>8</v>
       </c>
       <c r="J23" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="42">
+    <row r="24" spans="1:11">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="H24" s="11" t="s">
+      <c r="H24" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="14">
         <v>8</v>
       </c>
       <c r="J24" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="56">
+    <row r="25" spans="1:11">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="14">
         <v>9</v>
       </c>
       <c r="J25" t="s">
@@ -1673,7 +1844,7 @@
       <c r="H26" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="14">
         <v>113</v>
       </c>
       <c r="J26" s="2" t="s">
@@ -1702,36 +1873,43 @@
       <c r="F27" s="2" t="s">
         <v>137</v>
       </c>
+      <c r="G27" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I27" s="14">
+        <v>4</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>139</v>
-      </c>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="H28" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="I28" s="14">
+        <v>4</v>
+      </c>
+      <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>143</v>
@@ -1740,38 +1918,47 @@
         <v>144</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I29" s="14">
+        <v>173</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>140</v>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="H30" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="I30" s="14">
+        <v>173</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>143</v>
@@ -1780,15 +1967,15 @@
         <v>144</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>128</v>
@@ -1800,235 +1987,244 @@
         <v>144</v>
       </c>
       <c r="F32" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="2" t="s">
+    <row r="35" spans="1:11">
+      <c r="A35" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="D35" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:11">
       <c r="A36" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="I36" s="14">
+        <v>112</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="I37" s="14">
+        <v>112</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="I38" s="14">
+        <v>113</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="K38" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="I39" s="14">
+        <v>112</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F36" s="2" t="s">
+      <c r="D41" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="2" t="s">
+    <row r="42" spans="1:11">
+      <c r="A42" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F37" s="2" t="s">
+      <c r="D42" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="3" t="s">
+    <row r="43" spans="1:11">
+      <c r="A43" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F38" s="2" t="s">
+      <c r="D43" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="2" t="s">
+    <row r="44" spans="1:11">
+      <c r="A44" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>135</v>
@@ -2040,566 +2236,964 @@
         <v>143</v>
       </c>
       <c r="F44" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="I44" s="14">
+        <v>193</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="H45" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="I45" s="17">
+        <v>193</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="H46" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="I46" s="14">
+        <v>194</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="H47" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="I47" s="14">
+        <v>194</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="H48" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="I48" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="H49" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="I49" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="H50" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="I50" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="J50" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C45" s="2" t="s">
+      <c r="G51" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="I51" s="14">
+        <v>1040</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F46" s="2" t="s">
+      <c r="D53" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C47" s="2" t="s">
+      <c r="G53" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="I53" s="14">
+        <v>554</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="H54" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I54" s="14">
+        <v>554</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="H55" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="I55" s="14">
+        <v>554</v>
+      </c>
+      <c r="J55" t="s">
+        <v>226</v>
+      </c>
+      <c r="K55" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="H56" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="I56" s="14">
+        <v>554</v>
+      </c>
+      <c r="J56" t="s">
+        <v>226</v>
+      </c>
+      <c r="K56" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="H57" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="I57" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="J57" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="H58" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="I58" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="J58" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="H59" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="I59" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="J59" t="s">
+        <v>226</v>
+      </c>
+      <c r="K59" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="H60" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="I60" s="15"/>
+      <c r="J60" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="H61" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="I61" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="J61" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="H62" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="I62" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="J62" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F58" s="2" t="s">
+      <c r="D63" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F63" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
-      <c r="A59" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C61" s="2" t="s">
+    <row r="64" spans="1:11">
+      <c r="A64" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="D64" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="2" t="s">
-        <v>59</v>
+      <c r="A65" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>128</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="2" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>129</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>128</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="2" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="2" t="s">
-        <v>64</v>
+      <c r="A70" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>128</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="3" t="s">
-        <v>65</v>
+      <c r="A71" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="2" t="s">
-        <v>66</v>
+      <c r="A72" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>128</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F72" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F92" s="2" t="s">
         <v>137</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improved Learning Curve FTW!
1234
</commit_message>
<xml_diff>
--- a/Review.xlsx
+++ b/Review.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sven\Documents\GitHub\AR-Education\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-435" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="-435" windowWidth="28800" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="287">
   <si>
     <t>Title</t>
   </si>
@@ -562,9 +557,6 @@
   </si>
   <si>
     <t>Increased details</t>
-  </si>
-  <si>
-    <t>Improved spatial abilities</t>
   </si>
   <si>
     <t>"simulation environments could support students’ scientific inquiry learning processes, such as interpreting results, and improving knowledge integration"</t>
@@ -660,9 +652,6 @@
     <t xml:space="preserve">his supports the notion that AR books can help in learning complex three dimensional concepts </t>
   </si>
   <si>
-    <t>developmentof spatial abilities</t>
-  </si>
-  <si>
     <t>The interactivity afforded by AR books provides great potential for learning and an advantage over traditional books or other learning media. Tangible interaction using tools such as the magnet paddle and augmented nail with labeled poles allow for a learning experience that combines real world objects with virtual content. Together this can contribute to a deeper understanding. Interactions in AR engage learners with the content, and allow for knowledge to be acquired through their own manipulation of content (Dünser, 2008), as supported by constructivist learning theory (Tobias &amp; Duffy, 2009 ).</t>
   </si>
   <si>
@@ -677,9 +666,6 @@
     <t>Contibution to deeper understanding through interaction with a combination of real world objects and virtual content</t>
   </si>
   <si>
-    <t>deeper learning through the combination of real world objects and virtual content</t>
-  </si>
-  <si>
     <t>The AR-guided group had better learning effectiveness (as evidenced by their posttest scores), and it was found that most visitors believed the AR guide made it easier to digest information than the audio guide due to the extra visual commentary that is provided. This mode not only offers an audio commentary, but also displays visual information dominated by text and images.</t>
   </si>
   <si>
@@ -780,6 +766,197 @@
   </si>
   <si>
     <t>improved collaborative learning</t>
+  </si>
+  <si>
+    <t>Drinn?</t>
+  </si>
+  <si>
+    <t>Nein</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Anzahl Artikel</t>
+  </si>
+  <si>
+    <t>From the analysis of the nine factors underlying users’ flow experiences, the experimental group showed higher levels of concentration on the task (CT) and distorted sense of time (DT) than the control group, which might have led to the students achieving deep learning (Liu, Cheng, &amp; Huang, 2011).</t>
+  </si>
+  <si>
+    <t>Statistical results also show that the experimental group had a better sense of control (SC) and clearer direct feed- back (CF) than the control group, which can be beneficial for the recall of information, according to Bujak et al.’s (2013) study.</t>
+  </si>
+  <si>
+    <t>Finally, participants in the AR-based learning activity reported the highest levels of intrinsic satisfaction (AE) compared to those who used the web-based application; this may have helped the experimental group to perform the task more easily that the control group.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regarding the learning effectiveness of both applications, after conducting a statistical analysis on the pre- and posttest scores, it was found that students who used the AR application performed significantly better on knowledge than those who were taught using the web- based application. Those findings seem to support the outcomes of research studies (Andujar, Mejias, &amp; Marquez, 2011; Chen, Chi, Hung, &amp; Kang, 2011; Kamarainen et al., 2013; Kaufmann &amp; Schmalstieg, 2003; Lin, Duh, Li, Wang, &amp; Tsai, 2013), which showed that AR technology contributed to improve academic achievement compared to traditional teaching methods. </t>
+  </si>
+  <si>
+    <t>The AR-based application enabled students to experiment interactively with electric and magnetic fields as well as to observe the effect of magnetic forces on their circuit. It provided instant and reliable feedback.</t>
+  </si>
+  <si>
+    <t>Therefore, the AR-based application gave students the opportunity to try and observe different options instantly, whereas the web-based application did not offer students any possibility to experiment.</t>
+  </si>
+  <si>
+    <t>The experimental group experienced higher levels of concentration on tasks
+(M ¼ 4.02, SD ¼ 0.60) than the control group (M ¼ 3.49, SD ¼ 0.83) [t ¼ 2.771, df ¼ 58, p-value ¼ 0.008, d ¼ 0.87]. Furthermore, AR-based
+application users had a higher sense of control (M ¼ 3.79, SD ¼ 0.53) than web-based application users (M ¼ 3.42, SD ¼ 0.59) [t ¼  2.505,
+df ¼ 57.923, p-value ¼ 0.015, d ¼ 0.68]. Finally, the experimental group reported a higher distorted sense of time (M ¼ 3.37, SD ¼ 0.92) than the control group (M ¼ 2.85, SD ¼ 0.71) [t ¼  2.392, df ¼ 50.366, p-value ¼ 0.02, d ¼ 0.56] (see Fig. 5).</t>
+  </si>
+  <si>
+    <t>Results indicate
+that the experimental group had higher levels of clear and direct feedback factor (M ¼ 3.64, SD ¼ 0.48) than the control group (M ¼ 3.27,
+SD ¼ 0.64) [U ¼ 303.5, p-value ¼ 0.03, d ¼ 0.58]. Similarly, the experimental group had higher values of autotelic experience (M ¼ 4.20,
+SD ¼ 0.71) than the control group (M¼ 3.63, SD ¼ 0.69) [U ¼ 243.5, p-value ¼ 0.002, d ¼ 0.86] (see Fig. 6).</t>
+  </si>
+  <si>
+    <t>Results showed that students were less bored and more in flow state
+when the AR-based application was used during the Magnet_2 stage.</t>
+  </si>
+  <si>
+    <t>Results showed that there are differences in students’ learning outcomes depending on which of the two learning applications they used.
+Indeed, students using the AR-based application performed significantly higher in the posttest than those that had used the web-based
+application.</t>
+  </si>
+  <si>
+    <t>Fehlt</t>
+  </si>
+  <si>
+    <t>In this study, we investigated the impact of an AR- supported simulation on the effectiveness of face-to-face collaborative learning for Physics. The results demonstrated the facilitation effects of AR technology on collaborative learning effectiveness.</t>
+  </si>
+  <si>
+    <t>The collaborators with the AR-supported simulation perceived higher levels of learning skill development, self- reported learning and learning interest after the discussion compared with those without simulation support</t>
+  </si>
+  <si>
+    <t>The analysis indicated that the participants with the ARsupported
+simulation gave significantly higher ratings in
+perceived skill development than those in the non-ARsupported
+groups.</t>
+  </si>
+  <si>
+    <t>Individual post-test results showed that participants in the
+AR-supported groups got significantly higher scores than
+those in the non-AR-supported groups (See Table II).</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>The learning satisfaction of the experimental group learners was higher than that of the control group learners who received librarian instruction. Particularly, learner satisfaction assessed by questions 1 and 7 differed significantly between the two groups. These two questions asked learners whether using the proposed ARLIS for library instruction was more fun than librarian instruction?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nein </t>
+  </si>
+  <si>
+    <t>The training of spatial ability based on Graphic Engineering contents and AR technology improves spatial abilities for those who perform them and consequently lower the numbers of students who drop out of the subject.</t>
+  </si>
+  <si>
+    <t>" reached a satisfactory motivation level."</t>
+  </si>
+  <si>
+    <t>"positive performance"</t>
+  </si>
+  <si>
+    <t>Students have been satisfied and motivated by these new methodologies, in all cases.</t>
+  </si>
+  <si>
+    <t>Regarding the second research question, results showed that AR technology can help to improve student’s academic performance.</t>
+  </si>
+  <si>
+    <t>their graphic competences and space skills are increased in shorter learning periods,</t>
+  </si>
+  <si>
+    <t>Test results obtained from learning activities revealed that the experimental group achieved significantly more learning improvement than the control group did.</t>
+  </si>
+  <si>
+    <t>Further, the interview results reveal that, compared to traditional learning methods, the proposed EULER not only increases the motivation of students to learn and improves the effectiveness of learning</t>
+  </si>
+  <si>
+    <t>but it also improves student creativity and the ability to explore and absorb new knowledge and solve problems.</t>
+  </si>
+  <si>
+    <t>"can increase motivation to learn"</t>
+  </si>
+  <si>
+    <t>"can improve listening, speaking and reading ability."</t>
+  </si>
+  <si>
+    <t>"like to use the HELLO to learn after class."</t>
+  </si>
+  <si>
+    <t>The experimental results indicate that using the MDAS as a teaching tool for astronomical observations in an outdoor teaching envi- ronment enables students to achieve better learning achievements and to exhibit excellent skill performance</t>
+  </si>
+  <si>
+    <t>Students using the MDAS were significantly more active and engaged in interactions with the teacher compared to those students using traditional tools.</t>
+  </si>
+  <si>
+    <t>"enhanced the effectiveness of learning about astronomical observation and the performance of astronomical observation skills. In addition, the introduction of augmented reality to construct a human–computer-field experience sub- stantially increased learner motivation and had a stronger effect on the retention of learner interest in astronomical observation compared to traditional teaching scenarios."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Overlay system helped not only to avoid the initial period of high errors and lengthy procedures, but also improved overall accuracy and efficiency after the training session. </t>
+  </si>
+  <si>
+    <t>Therefore, it is likely that this method would decrease the amount of practice required for medical stu- dents to become eligible for clinical procedures, or to master percutaneous needle insertion technique.</t>
+  </si>
+  <si>
+    <t>"Potential tissue damage caused by the needle [see Fig. 7(b)] was lower in the Overlay group for all insertions, and it remained significantly lower when the group performed the freehand insertion."</t>
+  </si>
+  <si>
+    <t>"Success rate [see Fig. 7(c)] was higher in the Overlay group when receiving additional guidance for the first six insertions, and remained higher during the freehand insertions."</t>
+  </si>
+  <si>
+    <t>When trainees relied on their memory and the manual to complete an assembly, they were prone to making errors. When AR was used, the learning curve of trainees significantly improved, and fewer errors were made.</t>
+  </si>
+  <si>
+    <t>The use of an animated AR system as a training tool shortens the learning curve of trainees in cognition-demanded assembl</t>
+  </si>
+  <si>
+    <t>"AR is able to compensate for the mental and cognitive gaps between individual differences of information retrieval capacity and the task difficulty imposed on individuals. Consequently, AR eases information retrieval by integrating the task of searching information and the task of the actual assembly."</t>
+  </si>
+  <si>
+    <t>"AR appears to have an advantage in reduc- ing error assembly when compared with the assembly manual."</t>
+  </si>
+  <si>
+    <t>"average ratings of both frustration level and temporal demand were higher using the manual"</t>
+  </si>
+  <si>
+    <t>"Trainees with AR training could remember or recollect more assembly clues that were memorized in the former training task than those trained in the manual."</t>
+  </si>
+  <si>
+    <t>Simultaneous AR with the integration of human cadaver models can aid in decreasing the leaming curve to leam complex invasive procedures.</t>
+  </si>
+  <si>
+    <t>Overall, the students were quite satisfied with the tools used to learn.</t>
+  </si>
+  <si>
+    <t>According to the data observed on site, we note that students who trained using AR felt quite impressed and motivated by the use of a new technology, of which they had no previous contact as they were not aware of it.</t>
+  </si>
+  <si>
+    <t>The computer tools that allow virtual modeling and the handling of 3D objects ease teaching tasks as any piece or figure is available without needing to obtain physical models that can be quite expensive and take longer to create.</t>
+  </si>
+  <si>
+    <t>The groups that underwent training showed a statistically- significant improvement in spatial ability levels. P-values are around 5% for statistical significance, which indicates that the students have a probability of over 95% of improving their levels of spatial ability when performing the proposed training. Besides this, results show there is no improvement in control group levels.</t>
+  </si>
+  <si>
+    <t>"The retention scores show improved learning with YouMove, as performance is maintained on the retention tests"</t>
+  </si>
+  <si>
+    <t>Overall, we were pleased to see that when comparing pre- test and post-test results, learning increased by more than a factor of 2 (44% vs. 20%) with the YouMove system.</t>
+  </si>
+  <si>
+    <t>improved concentration</t>
+  </si>
+  <si>
+    <t>Higher level of satisfaction</t>
+  </si>
+  <si>
+    <t>deeper learning through the interactivity of real world objects and virtual content (Interactivity)</t>
+  </si>
+  <si>
+    <t>After class learning!</t>
+  </si>
+  <si>
+    <t>Improved memory</t>
   </si>
 </sst>
 </file>
@@ -902,7 +1079,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -937,6 +1114,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -949,16 +1129,16 @@
     <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1229,7 +1409,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1237,11 +1417,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K92"/>
+  <dimension ref="A1:L154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L132" sqref="L132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1256,7 +1436,7 @@
     <col min="10" max="10" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1290,8 +1470,11 @@
       <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="18" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1310,8 +1493,11 @@
       <c r="F2" s="6" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1345,8 +1531,11 @@
       <c r="K3" s="9" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1366,7 +1555,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1383,7 +1572,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1417,8 +1606,11 @@
       <c r="K6" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1437,8 +1629,11 @@
       <c r="F7" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -1457,8 +1652,11 @@
       <c r="F8" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
@@ -1477,8 +1675,11 @@
       <c r="F9" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1509,8 +1710,11 @@
       <c r="J10" s="2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1528,7 +1732,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1546,7 +1750,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1564,7 +1768,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1582,7 +1786,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
@@ -1613,8 +1817,11 @@
       <c r="J15" s="2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="L15" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1632,7 +1839,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:12">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1647,10 +1854,10 @@
         <v>5</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -1673,7 +1880,7 @@
         <v>142</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I18" s="14">
         <v>56</v>
@@ -1681,8 +1888,11 @@
       <c r="J18" s="2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1690,16 +1900,16 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I19" s="14">
         <v>5</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1718,8 +1928,11 @@
       <c r="F20" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -1742,16 +1955,19 @@
         <v>139</v>
       </c>
       <c r="H21" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="I21" s="15" t="s">
         <v>177</v>
-      </c>
-      <c r="I21" s="15" t="s">
-        <v>178</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="L21" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1774,7 +1990,7 @@
         <v>140</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I22" s="14">
         <v>8</v>
@@ -1782,8 +1998,11 @@
       <c r="J22" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="L22" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1791,16 +2010,16 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="H23" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I23" s="14">
         <v>8</v>
       </c>
       <c r="J23" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1808,16 +2027,16 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="H24" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I24" s="14">
         <v>8</v>
       </c>
       <c r="J24" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1825,7 +2044,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="H25" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I25" s="14">
         <v>9</v>
@@ -1834,7 +2053,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:12">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1842,7 +2061,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="H26" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I26" s="14">
         <v>113</v>
@@ -1851,10 +2070,10 @@
         <v>160</v>
       </c>
       <c r="K26" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="3" t="s">
         <v>21</v>
       </c>
@@ -1877,16 +2096,19 @@
         <v>137</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I27" s="14">
         <v>4</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+        <v>187</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1894,14 +2116,14 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="H28" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I28" s="14">
         <v>4</v>
       </c>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:12">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -1924,7 +2146,7 @@
         <v>139</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I29" s="14">
         <v>173</v>
@@ -1932,8 +2154,11 @@
       <c r="J29" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="L29" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1941,7 +2166,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="H30" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I30" s="14">
         <v>173</v>
@@ -1950,7 +2175,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:12">
       <c r="A31" s="2" t="s">
         <v>23</v>
       </c>
@@ -1969,8 +2194,11 @@
       <c r="F31" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="L31" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="2" t="s">
         <v>24</v>
       </c>
@@ -1989,8 +2217,11 @@
       <c r="F32" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="L32" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="2" t="s">
         <v>25</v>
       </c>
@@ -2009,8 +2240,11 @@
       <c r="F33" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="34" spans="1:11">
+      <c r="L33" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="2" t="s">
         <v>26</v>
       </c>
@@ -2029,8 +2263,11 @@
       <c r="F34" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="35" spans="1:11">
+      <c r="L34" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" s="2" t="s">
         <v>27</v>
       </c>
@@ -2049,8 +2286,11 @@
       <c r="F35" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="36" spans="1:11">
+      <c r="L35" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="2" t="s">
         <v>28</v>
       </c>
@@ -2073,16 +2313,19 @@
         <v>141</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I36" s="14">
         <v>112</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
+        <v>192</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2091,16 +2334,16 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I37" s="14">
         <v>112</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2109,19 +2352,19 @@
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I38" s="14">
         <v>113</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>200</v>
+        <v>284</v>
       </c>
       <c r="K38" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2130,16 +2373,16 @@
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I39" s="14">
         <v>112</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" s="3" t="s">
         <v>29</v>
       </c>
@@ -2158,8 +2401,11 @@
       <c r="F40" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="41" spans="1:11">
+      <c r="L40" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" s="2" t="s">
         <v>30</v>
       </c>
@@ -2178,8 +2424,11 @@
       <c r="F41" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="42" spans="1:11">
+      <c r="L41" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" s="2" t="s">
         <v>31</v>
       </c>
@@ -2198,8 +2447,11 @@
       <c r="F42" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="L42" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" s="3" t="s">
         <v>32</v>
       </c>
@@ -2218,8 +2470,11 @@
       <c r="F43" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="44" spans="1:11">
+      <c r="L43" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" s="2" t="s">
         <v>33</v>
       </c>
@@ -2242,7 +2497,7 @@
         <v>139</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="I44" s="14">
         <v>193</v>
@@ -2250,8 +2505,11 @@
       <c r="J44" s="2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="45" spans="1:11">
+      <c r="L44" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2259,16 +2517,16 @@
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="H45" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="I45" s="17">
         <v>193</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2276,16 +2534,16 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="H46" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I46" s="14">
         <v>194</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2293,16 +2551,16 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="H47" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I47" s="14">
         <v>194</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2310,16 +2568,16 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="H48" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:12">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2327,16 +2585,16 @@
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="H49" s="8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I49" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2344,16 +2602,16 @@
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="H50" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="I50" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J50" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:12">
       <c r="A51" s="2" t="s">
         <v>34</v>
       </c>
@@ -2376,7 +2634,7 @@
         <v>139</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="I51" s="14">
         <v>1040</v>
@@ -2384,8 +2642,11 @@
       <c r="J51" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="52" spans="1:11">
+      <c r="L51" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52" s="2" t="s">
         <v>35</v>
       </c>
@@ -2404,8 +2665,11 @@
       <c r="F52" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="53" spans="1:11">
+      <c r="L52" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
       <c r="A53" s="2" t="s">
         <v>36</v>
       </c>
@@ -2428,7 +2692,7 @@
         <v>139</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="I53" s="14">
         <v>554</v>
@@ -2436,8 +2700,11 @@
       <c r="J53" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="54" spans="1:11">
+      <c r="L53" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2445,16 +2712,16 @@
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="H54" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="I54" s="14">
         <v>554</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2462,19 +2729,19 @@
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="H55" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I55" s="14">
         <v>554</v>
       </c>
       <c r="J55" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="K55" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2482,19 +2749,19 @@
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="H56" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I56" s="14">
         <v>554</v>
       </c>
       <c r="J56" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="K56" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2502,16 +2769,16 @@
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="H57" s="8" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="I57" s="15" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="J57" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2519,16 +2786,16 @@
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="H58" s="8" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="I58" s="15" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J58" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2536,19 +2803,19 @@
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="H59" s="8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I59" s="15" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J59" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="K59" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2556,14 +2823,14 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="H60" s="8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I60" s="15"/>
       <c r="J60" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2571,16 +2838,16 @@
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="H61" s="8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I61" s="15" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J61" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2588,16 +2855,16 @@
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="H62" s="8" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I62" s="15" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="J62" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
       <c r="A63" s="5" t="s">
         <v>37</v>
       </c>
@@ -2616,8 +2883,11 @@
       <c r="F63" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="64" spans="1:11">
+      <c r="L63" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
       <c r="A64" s="2" t="s">
         <v>38</v>
       </c>
@@ -2636,436 +2906,460 @@
       <c r="F64" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="3" t="s">
+      <c r="G64" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="I64">
+        <v>11</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="H65" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="I65">
+        <v>11</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="H66" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="I66">
+        <v>11</v>
+      </c>
+      <c r="J66" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="H67" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="I67">
+        <v>12</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="H68" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="I68">
+        <v>12</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="H69" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="I69">
+        <v>12</v>
+      </c>
+      <c r="J69" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="H70" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="I70" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="H71" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="I71" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="H72" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="I72" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="H73" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="I73" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="J73" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
-      <c r="A74" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>128</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E74" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="L74" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D75" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F74" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
-      <c r="A75" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="E75" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
+        <v>139</v>
+      </c>
+      <c r="L75" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
       <c r="A76" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>128</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E76" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L76" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D77" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="E77" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C77" s="2" t="s">
+      <c r="L77" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="A78" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="I78">
+        <v>322</v>
+      </c>
+      <c r="J78" t="s">
+        <v>227</v>
+      </c>
+      <c r="L78" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="H79" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="I79">
+        <v>322</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="H80" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="I80">
+        <v>322</v>
+      </c>
+      <c r="J80" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="H81" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="I81" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="J81" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
+      <c r="A82" s="2"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="H82" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="I82" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="J82" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
+      <c r="A83" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E77" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F77" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
-      <c r="A80" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
-      <c r="A81" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
-      <c r="A82" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
-      <c r="A83" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="E83" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
-      <c r="A84" s="3" t="s">
-        <v>58</v>
+        <v>140</v>
+      </c>
+      <c r="L83" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
+      <c r="A84" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>129</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
-      <c r="A85" s="2" t="s">
-        <v>59</v>
+        <v>137</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="I84">
+        <v>649</v>
+      </c>
+      <c r="J84" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="L84" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
+      <c r="A85" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>128</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
+        <v>140</v>
+      </c>
+      <c r="L85" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
       <c r="A86" s="2" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>144</v>
@@ -3074,15 +3368,18 @@
         <v>145</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
+        <v>137</v>
+      </c>
+      <c r="L86" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
       <c r="A87" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>128</v>
@@ -3094,18 +3391,21 @@
         <v>145</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
+        <v>142</v>
+      </c>
+      <c r="L87" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
       <c r="A88" s="2" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>144</v>
@@ -3114,55 +3414,62 @@
         <v>145</v>
       </c>
       <c r="F88" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G88" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="89" spans="1:6">
-      <c r="A89" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
-      <c r="A90" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
-      <c r="A91" s="3" t="s">
-        <v>65</v>
+      <c r="H88" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I88" s="20"/>
+      <c r="J88" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="L88" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
+      <c r="A89" s="2"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="H89" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="I89">
+        <v>6</v>
+      </c>
+      <c r="J89" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
+      <c r="A90" s="2"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="H90" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="I90">
+        <v>6</v>
+      </c>
+      <c r="J90" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
+      <c r="A91" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>128</v>
@@ -3174,15 +3481,18 @@
         <v>145</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
+        <v>137</v>
+      </c>
+      <c r="L91" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
       <c r="A92" s="2" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>128</v>
@@ -3194,7 +3504,926 @@
         <v>145</v>
       </c>
       <c r="F92" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="I92">
+        <v>60</v>
+      </c>
+      <c r="J92" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="L92" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
+      <c r="A93" s="2"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="I93">
+        <v>60</v>
+      </c>
+      <c r="J93" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
+      <c r="A94" s="2"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="H94" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="I94">
+        <v>60</v>
+      </c>
+      <c r="J94" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
+      <c r="A95" s="2"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="H95" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="I95">
+        <v>60</v>
+      </c>
+      <c r="J95" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
+      <c r="A96" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="I96">
+        <v>173</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="L96" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
+      <c r="A97" s="2"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+      <c r="H97" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="I97">
+        <v>173</v>
+      </c>
+      <c r="J97" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
+      <c r="A98" s="2"/>
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+      <c r="H98" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="I98">
+        <v>173</v>
+      </c>
+      <c r="J98" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
+      <c r="A99" s="2"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+      <c r="H99" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="I99">
+        <v>173</v>
+      </c>
+      <c r="J99" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
+      <c r="A100" s="2"/>
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+      <c r="H100" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="I100">
+        <v>5</v>
+      </c>
+      <c r="J100" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
+      <c r="A101" s="2"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="H101" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="I101">
+        <v>5</v>
+      </c>
+      <c r="J101" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
+      <c r="A102" s="2"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="H102" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="I102">
+        <v>5</v>
+      </c>
+      <c r="J102" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="K102" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12">
+      <c r="A103" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="L103" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12">
+      <c r="A104" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L104" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12">
+      <c r="A105" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="I105"/>
+      <c r="J105" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="L105" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12">
+      <c r="A106" s="2"/>
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+      <c r="H106" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I106"/>
+      <c r="J106" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12">
+      <c r="A107" s="2"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
+      <c r="H107" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="I107">
+        <v>187</v>
+      </c>
+      <c r="J107" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12">
+      <c r="A108" s="2"/>
+      <c r="B108" s="2"/>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+      <c r="H108" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="I108">
+        <v>187</v>
+      </c>
+      <c r="J108" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12">
+      <c r="A109" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F109" s="2" t="s">
         <v>137</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="I109">
+        <v>2035</v>
+      </c>
+      <c r="J109" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="L109" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12">
+      <c r="A110" s="2"/>
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+      <c r="G110" s="2"/>
+      <c r="H110" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="I110">
+        <v>2035</v>
+      </c>
+      <c r="J110" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12">
+      <c r="A111" s="2"/>
+      <c r="B111" s="2"/>
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
+      <c r="G111" s="2"/>
+      <c r="H111" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="I111">
+        <v>2035</v>
+      </c>
+      <c r="J111" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12">
+      <c r="A112" s="2"/>
+      <c r="B112" s="2"/>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2"/>
+      <c r="G112" s="2"/>
+      <c r="H112" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="I112">
+        <v>2035</v>
+      </c>
+      <c r="J112" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12">
+      <c r="A113" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="L113" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12">
+      <c r="A114" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="L114" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12">
+      <c r="A115" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H115" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="I115">
+        <v>451</v>
+      </c>
+      <c r="J115" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="L115" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12">
+      <c r="A116" s="2"/>
+      <c r="B116" s="2"/>
+      <c r="C116" s="2"/>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="I116">
+        <v>450</v>
+      </c>
+      <c r="J116" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12">
+      <c r="A117" s="2"/>
+      <c r="B117" s="2"/>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
+      <c r="H117" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="I117">
+        <v>447</v>
+      </c>
+      <c r="J117" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12">
+      <c r="A118" s="2"/>
+      <c r="B118" s="2"/>
+      <c r="C118" s="2"/>
+      <c r="D118" s="2"/>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2"/>
+      <c r="G118" s="2"/>
+      <c r="H118" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="I118">
+        <v>448</v>
+      </c>
+      <c r="J118" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12">
+      <c r="A119" s="2"/>
+      <c r="B119" s="2"/>
+      <c r="C119" s="2"/>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+      <c r="G119" s="2"/>
+      <c r="H119" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="I119">
+        <v>448</v>
+      </c>
+      <c r="J119" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12">
+      <c r="A120" s="2"/>
+      <c r="B120" s="2"/>
+      <c r="C120" s="2"/>
+      <c r="D120" s="2"/>
+      <c r="E120" s="2"/>
+      <c r="F120" s="2"/>
+      <c r="G120" s="2"/>
+      <c r="H120" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="I120">
+        <v>448</v>
+      </c>
+      <c r="J120" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12">
+      <c r="A121" s="2"/>
+      <c r="B121" s="2"/>
+      <c r="C121" s="2"/>
+      <c r="D121" s="2"/>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2"/>
+      <c r="G121" s="2"/>
+      <c r="H121" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="I121">
+        <v>450</v>
+      </c>
+      <c r="J121" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12">
+      <c r="A122" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="L122" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12">
+      <c r="A123" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H123" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="I123">
+        <v>984</v>
+      </c>
+      <c r="J123" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="L123" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12">
+      <c r="A124" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="L124" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12">
+      <c r="A125" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="L125" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12">
+      <c r="A126" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G126" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H126" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="I126"/>
+      <c r="J126" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="L126" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12">
+      <c r="A127" s="2"/>
+      <c r="B127" s="2"/>
+      <c r="C127" s="2"/>
+      <c r="D127" s="2"/>
+      <c r="E127" s="2"/>
+      <c r="F127" s="2"/>
+      <c r="G127" s="2"/>
+      <c r="H127" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="I127"/>
+      <c r="J127" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12">
+      <c r="A128" s="2"/>
+      <c r="B128" s="2"/>
+      <c r="C128" s="2"/>
+      <c r="D128" s="2"/>
+      <c r="E128" s="2"/>
+      <c r="F128" s="2"/>
+      <c r="G128" s="2"/>
+      <c r="H128" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="I128"/>
+      <c r="J128" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12">
+      <c r="A129" s="2"/>
+      <c r="B129" s="2"/>
+      <c r="C129" s="2"/>
+      <c r="D129" s="2"/>
+      <c r="E129" s="2"/>
+      <c r="F129" s="2"/>
+      <c r="G129" s="2"/>
+      <c r="H129" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="I129"/>
+      <c r="J129" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12">
+      <c r="A130" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="L130" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12">
+      <c r="A131" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H131" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I131">
+        <v>318</v>
+      </c>
+      <c r="J131" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="L131" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12">
+      <c r="H132" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="I132"/>
+      <c r="J132" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12">
+      <c r="K139" t="s">
+        <v>231</v>
+      </c>
+      <c r="L139">
+        <f>COUNTIF(L2:L131, "Ja")</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" t="s">
+        <v>137</v>
+      </c>
+      <c r="B150">
+        <f>COUNTIF(G:G, A150)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
+        <v>142</v>
+      </c>
+      <c r="B151">
+        <f>COUNTIF(G:G, A151)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" t="s">
+        <v>140</v>
+      </c>
+      <c r="B152">
+        <f>COUNTIF(G:G, A152)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" t="s">
+        <v>141</v>
+      </c>
+      <c r="B153">
+        <f>COUNTIF(G:G, A153)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" t="s">
+        <v>139</v>
+      </c>
+      <c r="B154">
+        <f>COUNTIF(G:G, A154)</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inter Coder Reliability Vorbereitung
</commit_message>
<xml_diff>
--- a/Review.xlsx
+++ b/Review.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24709"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16080" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16080"/>
   </bookViews>
   <sheets>
     <sheet name="Gefiltert" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="307">
   <si>
     <t>Title</t>
   </si>
@@ -1005,6 +1005,21 @@
   </si>
   <si>
     <t>Gesamt</t>
+  </si>
+  <si>
+    <t>Passt?</t>
+  </si>
+  <si>
+    <t>Anzahl Fälle</t>
+  </si>
+  <si>
+    <t>Anzahl passend</t>
+  </si>
+  <si>
+    <t>Anzahl nicht passend</t>
+  </si>
+  <si>
+    <t>Intercoder Reliability</t>
   </si>
 </sst>
 </file>
@@ -1203,8 +1218,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="129">
+  <cellStyleXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1396,7 +1421,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="129">
+  <cellStyles count="139">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -1461,6 +1486,11 @@
     <cellStyle name="Besuchter Link" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1525,6 +1555,11 @@
     <cellStyle name="Link" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1800,7 +1835,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1808,11 +1843,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N120"/>
+  <dimension ref="A1:O120"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G117" sqref="G117"/>
+      <selection pane="bottomLeft" activeCell="G102" sqref="G102:H105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1820,14 +1855,14 @@
     <col min="1" max="1" width="23.1640625" customWidth="1"/>
     <col min="4" max="4" width="36.1640625" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="16.1640625" customWidth="1"/>
-    <col min="9" max="9" width="57" style="8" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="14"/>
-    <col min="11" max="12" width="39.6640625" customWidth="1"/>
+    <col min="6" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" customWidth="1"/>
+    <col min="10" max="10" width="57" style="8" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="14"/>
+    <col min="12" max="13" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1850,26 +1885,29 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="1"/>
+      <c r="N1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="O1" s="18" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1891,29 +1929,33 @@
       <c r="G2" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="6" t="b">
+        <f>EXACT(F2,G2)</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="K2" s="15" t="s">
         <v>151</v>
-      </c>
-      <c r="K2" t="s">
-        <v>225</v>
       </c>
       <c r="L2" t="s">
         <v>225</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" t="s">
+        <v>225</v>
+      </c>
+      <c r="N2" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1921,26 +1963,27 @@
       <c r="E3" s="2"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="J3" s="16">
+      <c r="K3" s="16">
         <v>253</v>
-      </c>
-      <c r="K3" t="s">
-        <v>153</v>
       </c>
       <c r="L3" t="s">
         <v>153</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" t="s">
+        <v>153</v>
+      </c>
+      <c r="N3" s="7" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1948,21 +1991,22 @@
       <c r="E4" s="2"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="J4" s="16">
+      <c r="K4" s="16">
         <v>254</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="L4" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="L4" s="7"/>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="M4" s="7"/>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1984,29 +2028,33 @@
       <c r="G5" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="6" t="b">
+        <f>EXACT(F5,G5)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="J5" s="14">
+      <c r="K5" s="14">
         <v>525</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>154</v>
       </c>
       <c r="L5" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="N5" t="s">
         <v>156</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -2028,26 +2076,30 @@
       <c r="G6" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="6" t="b">
+        <f>EXACT(F6,G6)</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="J6" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="K6" s="15" t="s">
         <v>157</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="N6" t="s">
+      <c r="M6" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="O6" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2055,23 +2107,24 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="J7" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="K7" s="15" t="s">
         <v>157</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>297</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="M7" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2079,23 +2132,24 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="J8" s="15" t="s">
+      <c r="K8" s="15" t="s">
         <v>157</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="M8" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2103,23 +2157,24 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="2"/>
+      <c r="I9" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="J9" s="14">
+      <c r="K9" s="14">
         <v>894</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="M9" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2127,23 +2182,24 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="2"/>
+      <c r="I10" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="J10" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="J10" s="14">
+      <c r="K10" s="14">
         <v>894</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="M10" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -2165,26 +2221,30 @@
       <c r="G11" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="6" t="b">
+        <f>EXACT(F11,G11)</f>
+        <v>1</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="J11" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="K11" s="15" t="s">
         <v>157</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="N11" t="s">
+      <c r="M11" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="O11" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2192,23 +2252,24 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="2"/>
+      <c r="I12" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="J12" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="J12" s="15" t="s">
+      <c r="K12" s="15" t="s">
         <v>168</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="M12" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2216,23 +2277,24 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="J13" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="J13" s="14">
+      <c r="K13" s="14">
         <v>5</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="M13" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -2254,26 +2316,30 @@
       <c r="G14" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="6" t="b">
+        <f>EXACT(F14,G14)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J14" s="14">
+      <c r="K14" s="14">
         <v>56</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="M14" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="O14" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:15">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2281,23 +2347,24 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="J15" s="14">
+      <c r="K15" s="14">
         <v>5</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>174</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="M15" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -2319,26 +2386,30 @@
       <c r="G16" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="6" t="b">
+        <f>EXACT(F16,G16)</f>
+        <v>1</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="J16" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="J16" s="15" t="s">
+      <c r="K16" s="15" t="s">
         <v>176</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="N16" t="s">
+      <c r="M16" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="O16" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:15">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -2360,26 +2431,30 @@
       <c r="G17" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="6" t="b">
+        <f>EXACT(F17,G17)</f>
+        <v>1</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="J17" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="J17" s="14">
+      <c r="K17" s="14">
         <v>8</v>
-      </c>
-      <c r="K17" t="s">
-        <v>159</v>
       </c>
       <c r="L17" t="s">
         <v>159</v>
       </c>
-      <c r="N17" t="s">
+      <c r="M17" t="s">
+        <v>159</v>
+      </c>
+      <c r="O17" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:15">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2387,23 +2462,24 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="2"/>
+      <c r="I18" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="J18" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="J18" s="14">
+      <c r="K18" s="14">
         <v>8</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="M18" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2411,23 +2487,24 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="2"/>
+      <c r="I19" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="J19" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="J19" s="14">
+      <c r="K19" s="14">
         <v>8</v>
-      </c>
-      <c r="K19" t="s">
-        <v>183</v>
       </c>
       <c r="L19" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="M19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2435,20 +2512,21 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="2"/>
+      <c r="I20" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="J20" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="J20" s="14">
+      <c r="K20" s="14">
         <v>9</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="L20" s="2" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:15">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2456,24 +2534,25 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="2"/>
+      <c r="I21" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="J21" s="14">
+      <c r="K21" s="14">
         <v>113</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="L21" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="L21" s="2"/>
-      <c r="M21" t="s">
+      <c r="M21" s="2"/>
+      <c r="N21" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:15">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -2495,26 +2574,30 @@
       <c r="G22" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="6" t="b">
+        <f>EXACT(F22,G22)</f>
+        <v>1</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="J22" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="J22" s="14">
+      <c r="K22" s="14">
         <v>4</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="N22" s="2" t="s">
+      <c r="M22" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="O22" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:15">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2522,21 +2605,22 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="2"/>
+      <c r="I23" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="J23" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="J23" s="14">
+      <c r="K23" s="14">
         <v>4</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="L23" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="L23" s="2"/>
-    </row>
-    <row r="24" spans="1:14">
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -2558,26 +2642,30 @@
       <c r="G24" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" s="6" t="b">
+        <f>EXACT(F24,G24)</f>
+        <v>1</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="J24" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="J24" s="14">
+      <c r="K24" s="14">
         <v>173</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="N24" s="2" t="s">
+      <c r="M24" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="O24" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:15">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2585,23 +2673,24 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="2"/>
+      <c r="I25" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="J25" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="J25" s="14">
+      <c r="K25" s="14">
         <v>173</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="M25" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
@@ -2623,26 +2712,30 @@
       <c r="G26" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H26" s="6" t="b">
+        <f>EXACT(F26,G26)</f>
+        <v>1</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="J26" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="J26" s="14">
+      <c r="K26" s="14">
         <v>112</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="N26" s="2" t="s">
+      <c r="M26" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="O26" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:15">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2650,21 +2743,22 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="2" t="s">
+      <c r="H27" s="2"/>
+      <c r="I27" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="I27" s="12" t="s">
+      <c r="J27" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="J27" s="14">
+      <c r="K27" s="14">
         <v>112</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="L27" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="L27" s="2"/>
-    </row>
-    <row r="28" spans="1:14">
+      <c r="M27" s="2"/>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2672,26 +2766,27 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="2" t="s">
+      <c r="H28" s="2"/>
+      <c r="I28" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="I28" s="12" t="s">
+      <c r="J28" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="J28" s="14">
+      <c r="K28" s="14">
         <v>113</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>294</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="M28" t="s">
+      <c r="M28" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="N28" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:15">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2699,23 +2794,24 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="2" t="s">
+      <c r="H29" s="2"/>
+      <c r="I29" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="I29" s="12" t="s">
+      <c r="J29" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="J29" s="14">
+      <c r="K29" s="14">
         <v>112</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="M29" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
@@ -2737,26 +2833,30 @@
       <c r="G30" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" s="6" t="b">
+        <f>EXACT(F30,G30)</f>
+        <v>1</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="J30" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="J30" s="14">
+      <c r="K30" s="14">
         <v>193</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="N30" s="2" t="s">
+      <c r="M30" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="O30" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:15">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2764,23 +2864,24 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="2" t="s">
+      <c r="H31" s="2"/>
+      <c r="I31" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="J31" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="J31" s="17">
+      <c r="K31" s="17">
         <v>193</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="32" spans="1:14">
+      <c r="M31" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2788,23 +2889,24 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="2" t="s">
+      <c r="H32" s="2"/>
+      <c r="I32" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="J32" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="J32" s="14">
+      <c r="K32" s="14">
         <v>194</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="33" spans="1:14">
+      <c r="M32" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2812,23 +2914,24 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="2" t="s">
+      <c r="H33" s="2"/>
+      <c r="I33" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="J33" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="J33" s="14">
+      <c r="K33" s="14">
         <v>194</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>297</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="34" spans="1:14">
+      <c r="M33" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2836,21 +2939,22 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="2" t="s">
+      <c r="H34" s="2"/>
+      <c r="I34" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I34" s="8" t="s">
+      <c r="J34" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="J34" s="15" t="s">
+      <c r="K34" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="K34" s="2" t="s">
+      <c r="L34" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="L34" s="2"/>
-    </row>
-    <row r="35" spans="1:14">
+      <c r="M34" s="2"/>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2858,21 +2962,22 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="2" t="s">
+      <c r="H35" s="2"/>
+      <c r="I35" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="J35" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="J35" s="15" t="s">
+      <c r="K35" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="K35" s="2" t="s">
+      <c r="L35" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="L35" s="2"/>
-    </row>
-    <row r="36" spans="1:14">
+      <c r="M35" s="2"/>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2880,23 +2985,24 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="2" t="s">
+      <c r="H36" s="2"/>
+      <c r="I36" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I36" s="8" t="s">
+      <c r="J36" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="J36" s="15" t="s">
+      <c r="K36" s="15" t="s">
         <v>206</v>
-      </c>
-      <c r="K36" t="s">
-        <v>159</v>
       </c>
       <c r="L36" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="37" spans="1:14">
+      <c r="M36" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" s="2" t="s">
         <v>34</v>
       </c>
@@ -2918,26 +3024,30 @@
       <c r="G37" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="H37" s="6" t="b">
+        <f>EXACT(F37,G37)</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I37" s="2" t="s">
+      <c r="J37" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="J37" s="14">
+      <c r="K37" s="14">
         <v>1040</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="N37" s="2" t="s">
+      <c r="M37" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="O37" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:15">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
@@ -2959,26 +3069,30 @@
       <c r="G38" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" s="6" t="b">
+        <f>EXACT(F38,G38)</f>
+        <v>1</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I38" s="2" t="s">
+      <c r="J38" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="J38" s="14">
+      <c r="K38" s="14">
         <v>554</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="L38" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="N38" s="2" t="s">
+      <c r="M38" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="O38" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:15">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2986,26 +3100,27 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-      <c r="H39" s="2" t="s">
+      <c r="H39" s="2"/>
+      <c r="I39" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="J39" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="J39" s="14">
+      <c r="K39" s="14">
         <v>554</v>
-      </c>
-      <c r="K39" t="s">
-        <v>222</v>
       </c>
       <c r="L39" t="s">
         <v>222</v>
       </c>
       <c r="M39" t="s">
+        <v>222</v>
+      </c>
+      <c r="N39" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:15">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -3013,23 +3128,24 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="2" t="s">
+      <c r="H40" s="2"/>
+      <c r="I40" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="J40" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="J40" s="14">
+      <c r="K40" s="14">
         <v>554</v>
       </c>
-      <c r="K40" t="s">
+      <c r="L40" t="s">
         <v>222</v>
       </c>
-      <c r="M40" t="s">
+      <c r="N40" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:15">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -3037,23 +3153,24 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
-      <c r="H41" s="2" t="s">
+      <c r="H41" s="2"/>
+      <c r="I41" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I41" s="8" t="s">
+      <c r="J41" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="J41" s="15" t="s">
+      <c r="K41" s="15" t="s">
         <v>201</v>
-      </c>
-      <c r="K41" t="s">
-        <v>225</v>
       </c>
       <c r="L41" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="42" spans="1:14">
+      <c r="M41" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -3061,23 +3178,24 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
-      <c r="H42" s="2" t="s">
+      <c r="H42" s="2"/>
+      <c r="I42" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I42" s="8" t="s">
+      <c r="J42" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="J42" s="15" t="s">
+      <c r="K42" s="15" t="s">
         <v>204</v>
-      </c>
-      <c r="K42" t="s">
-        <v>182</v>
       </c>
       <c r="L42" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="43" spans="1:14">
+      <c r="M42" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -3085,23 +3203,24 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
-      <c r="H43" s="2" t="s">
+      <c r="H43" s="2"/>
+      <c r="I43" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I43" s="8" t="s">
+      <c r="J43" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="J43" s="15" t="s">
+      <c r="K43" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
         <v>222</v>
       </c>
-      <c r="M43" t="s">
+      <c r="N43" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:15">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -3109,21 +3228,22 @@
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
-      <c r="H44" s="2" t="s">
+      <c r="H44" s="2"/>
+      <c r="I44" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I44" s="8" t="s">
+      <c r="J44" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="J44" s="15"/>
-      <c r="K44" t="s">
-        <v>226</v>
-      </c>
+      <c r="K44" s="15"/>
       <c r="L44" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="45" spans="1:14">
+      <c r="M44" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -3131,20 +3251,21 @@
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
-      <c r="H45" s="2" t="s">
+      <c r="H45" s="2"/>
+      <c r="I45" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I45" s="8" t="s">
+      <c r="J45" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="J45" s="15" t="s">
+      <c r="K45" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="K45" t="s">
+      <c r="L45" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:15">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -3152,20 +3273,21 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
-      <c r="H46" s="2" t="s">
+      <c r="H46" s="2"/>
+      <c r="I46" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I46" s="8" t="s">
+      <c r="J46" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="J46" s="15" t="s">
+      <c r="K46" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="K46" t="s">
+      <c r="L46" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:15">
       <c r="A47" s="2" t="s">
         <v>38</v>
       </c>
@@ -3184,53 +3306,58 @@
       <c r="F47" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2" t="s">
+      <c r="G47" s="2" t="s">
         <v>139</v>
       </c>
+      <c r="H47" s="6" t="b">
+        <f>EXACT(F47,G47)</f>
+        <v>0</v>
+      </c>
       <c r="I47" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J47" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="J47">
+      <c r="K47">
         <v>11</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="L47" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="N47" s="2" t="s">
+      <c r="M47" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="O47" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:15">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
-      <c r="G48" s="2" t="s">
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H48" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="I48" s="2" t="s">
+      <c r="J48" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>11</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>294</v>
       </c>
       <c r="L48" s="2" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="49" spans="1:14">
+      <c r="M48" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -3238,23 +3365,24 @@
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
-      <c r="H49" s="2" t="s">
+      <c r="H49" s="2"/>
+      <c r="I49" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I49" s="2" t="s">
+      <c r="J49" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="J49">
+      <c r="K49">
         <v>11</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>296</v>
       </c>
       <c r="L49" s="2" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="50" spans="1:14">
+      <c r="M49" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -3262,23 +3390,24 @@
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-      <c r="H50" s="2" t="s">
+      <c r="H50" s="2"/>
+      <c r="I50" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I50" s="2" t="s">
+      <c r="J50" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="J50">
+      <c r="K50">
         <v>12</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="L50" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="51" spans="1:14">
+      <c r="M50" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -3286,21 +3415,22 @@
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-      <c r="H51" s="2" t="s">
+      <c r="H51" s="2"/>
+      <c r="I51" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I51" s="2" t="s">
+      <c r="J51" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <v>12</v>
       </c>
-      <c r="K51" s="2" t="s">
+      <c r="L51" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="L51" s="2"/>
-    </row>
-    <row r="52" spans="1:14">
+      <c r="M51" s="2"/>
+    </row>
+    <row r="52" spans="1:15">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -3308,21 +3438,22 @@
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
-      <c r="H52" s="2" t="s">
+      <c r="H52" s="2"/>
+      <c r="I52" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I52" s="2" t="s">
+      <c r="J52" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="J52">
+      <c r="K52">
         <v>12</v>
       </c>
-      <c r="K52" s="2" t="s">
+      <c r="L52" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="L52" s="2"/>
-    </row>
-    <row r="53" spans="1:14">
+      <c r="M52" s="2"/>
+    </row>
+    <row r="53" spans="1:15">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -3330,21 +3461,22 @@
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
-      <c r="H53" s="2" t="s">
+      <c r="H53" s="2"/>
+      <c r="I53" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I53" s="8" t="s">
+      <c r="J53" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="J53" s="19" t="s">
+      <c r="K53" s="19" t="s">
         <v>203</v>
       </c>
-      <c r="K53" s="2" t="s">
+      <c r="L53" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="L53" s="2"/>
-    </row>
-    <row r="54" spans="1:14">
+      <c r="M53" s="2"/>
+    </row>
+    <row r="54" spans="1:15">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -3352,21 +3484,22 @@
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
-      <c r="H54" s="2" t="s">
+      <c r="H54" s="2"/>
+      <c r="I54" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I54" s="8" t="s">
+      <c r="J54" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="J54" s="19" t="s">
+      <c r="K54" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="K54" s="2" t="s">
+      <c r="L54" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="L54" s="2"/>
-    </row>
-    <row r="55" spans="1:14">
+      <c r="M54" s="2"/>
+    </row>
+    <row r="55" spans="1:15">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -3374,23 +3507,24 @@
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
-      <c r="H55" s="2" t="s">
+      <c r="H55" s="2"/>
+      <c r="I55" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I55" s="8" t="s">
+      <c r="J55" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="J55" s="19" t="s">
+      <c r="K55" s="19" t="s">
         <v>204</v>
-      </c>
-      <c r="K55" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="L55" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="56" spans="1:14">
+      <c r="M55" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -3398,21 +3532,22 @@
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
-      <c r="H56" s="2" t="s">
+      <c r="H56" s="2"/>
+      <c r="I56" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I56" s="8" t="s">
+      <c r="J56" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="J56" s="19" t="s">
+      <c r="K56" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="K56" s="2" t="s">
+      <c r="L56" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="L56" s="2"/>
-    </row>
-    <row r="57" spans="1:14">
+      <c r="M56" s="2"/>
+    </row>
+    <row r="57" spans="1:15">
       <c r="A57" s="2" t="s">
         <v>43</v>
       </c>
@@ -3431,53 +3566,58 @@
       <c r="F57" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2" t="s">
+      <c r="G57" s="2" t="s">
         <v>142</v>
       </c>
+      <c r="H57" s="6" t="b">
+        <f>EXACT(F57,G57)</f>
+        <v>0</v>
+      </c>
       <c r="I57" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J57" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="J57">
+      <c r="K57">
         <v>322</v>
-      </c>
-      <c r="K57" t="s">
-        <v>226</v>
       </c>
       <c r="L57" t="s">
         <v>226</v>
       </c>
-      <c r="N57" t="s">
+      <c r="M57" t="s">
+        <v>226</v>
+      </c>
+      <c r="O57" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:15">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
-      <c r="G58" s="2" t="s">
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="H58" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="I58" s="2" t="s">
+      <c r="J58" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="J58">
+      <c r="K58">
         <v>322</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="59" spans="1:14">
+      <c r="M58" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -3485,23 +3625,24 @@
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
-      <c r="H59" s="2" t="s">
+      <c r="H59" s="2"/>
+      <c r="I59" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I59" s="2" t="s">
+      <c r="J59" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="J59">
+      <c r="K59">
         <v>322</v>
-      </c>
-      <c r="K59" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="60" spans="1:14">
+      <c r="M59" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -3509,20 +3650,21 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
-      <c r="H60" s="2" t="s">
+      <c r="H60" s="2"/>
+      <c r="I60" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I60" s="8" t="s">
+      <c r="J60" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="J60" s="19" t="s">
+      <c r="K60" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="K60" t="s">
+      <c r="L60" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:15">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -3530,20 +3672,21 @@
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
-      <c r="H61" s="2" t="s">
+      <c r="H61" s="2"/>
+      <c r="I61" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I61" s="8" t="s">
+      <c r="J61" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="J61" s="19" t="s">
+      <c r="K61" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="K61" t="s">
+      <c r="L61" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:15">
       <c r="A62" s="2" t="s">
         <v>45</v>
       </c>
@@ -3562,27 +3705,33 @@
       <c r="F62" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G62" s="2"/>
-      <c r="H62" s="2" t="s">
+      <c r="G62" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="H62" s="6" t="b">
+        <f>EXACT(F62,G62)</f>
+        <v>0</v>
+      </c>
       <c r="I62" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J62" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="J62">
+      <c r="K62">
         <v>649</v>
-      </c>
-      <c r="K62" s="2" t="s">
-        <v>296</v>
       </c>
       <c r="L62" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="N62" t="s">
+      <c r="M62" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="O62" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:15">
       <c r="A63" s="2" t="s">
         <v>49</v>
       </c>
@@ -3602,52 +3751,55 @@
         <v>137</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="H63" s="2" t="s">
         <v>142</v>
       </c>
+      <c r="H63" s="6" t="b">
+        <f>EXACT(F63,G63)</f>
+        <v>0</v>
+      </c>
       <c r="I63" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J63" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="J63" s="20"/>
-      <c r="K63" s="2" t="s">
-        <v>191</v>
-      </c>
+      <c r="K63" s="20"/>
       <c r="L63" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="N63" t="s">
+      <c r="M63" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="O63" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:15">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
-      <c r="G64" s="2" t="s">
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="H64" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="I64" s="2" t="s">
+      <c r="J64" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="J64">
+      <c r="K64">
         <v>6</v>
-      </c>
-      <c r="K64" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="L64" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="65" spans="1:14">
+      <c r="M64" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -3655,23 +3807,24 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
-      <c r="H65" s="2" t="s">
+      <c r="H65" s="2"/>
+      <c r="I65" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I65" s="2" t="s">
+      <c r="J65" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="J65">
+      <c r="K65">
         <v>6</v>
-      </c>
-      <c r="K65" t="s">
-        <v>225</v>
       </c>
       <c r="L65" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="66" spans="1:14">
+      <c r="M65" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
       <c r="A66" s="2" t="s">
         <v>51</v>
       </c>
@@ -3690,53 +3843,58 @@
       <c r="F66" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2" t="s">
+      <c r="G66" s="2" t="s">
         <v>142</v>
       </c>
+      <c r="H66" s="6" t="b">
+        <f>EXACT(F66,G66)</f>
+        <v>1</v>
+      </c>
       <c r="I66" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J66" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="J66">
+      <c r="K66">
         <v>60</v>
-      </c>
-      <c r="K66" s="2" t="s">
-        <v>296</v>
       </c>
       <c r="L66" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="N66" t="s">
+      <c r="M66" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="O66" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="67" spans="1:14">
+    <row r="67" spans="1:15">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
-      <c r="G67" s="2" t="s">
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="H67" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="I67" s="2" t="s">
+      <c r="J67" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="J67">
+      <c r="K67">
         <v>60</v>
-      </c>
-      <c r="K67" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="68" spans="1:14">
+      <c r="M67" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -3744,23 +3902,24 @@
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
-      <c r="H68" s="2" t="s">
+      <c r="H68" s="2"/>
+      <c r="I68" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I68" s="2" t="s">
+      <c r="J68" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="J68">
+      <c r="K68">
         <v>60</v>
-      </c>
-      <c r="K68" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="L68" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="69" spans="1:14">
+      <c r="M68" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -3768,21 +3927,22 @@
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
-      <c r="H69" s="2" t="s">
+      <c r="H69" s="2"/>
+      <c r="I69" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I69" s="2" t="s">
+      <c r="J69" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="J69">
+      <c r="K69">
         <v>60</v>
       </c>
-      <c r="K69" s="2" t="s">
+      <c r="L69" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="L69" s="2"/>
-    </row>
-    <row r="70" spans="1:14">
+      <c r="M69" s="2"/>
+    </row>
+    <row r="70" spans="1:15">
       <c r="A70" s="2" t="s">
         <v>52</v>
       </c>
@@ -3801,53 +3961,58 @@
       <c r="F70" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="G70" s="2"/>
-      <c r="H70" s="2" t="s">
+      <c r="G70" s="2" t="s">
         <v>139</v>
       </c>
+      <c r="H70" s="6" t="b">
+        <f>EXACT(F70,G70)</f>
+        <v>1</v>
+      </c>
       <c r="I70" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J70" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="J70">
+      <c r="K70">
         <v>173</v>
-      </c>
-      <c r="K70" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="N70" s="2" t="s">
+      <c r="M70" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="O70" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:15">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
-      <c r="G71" s="2" t="s">
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H71" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="I71" s="2" t="s">
+      <c r="J71" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="J71">
+      <c r="K71">
         <v>173</v>
-      </c>
-      <c r="K71" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="72" spans="1:14">
+      <c r="M71" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -3855,23 +4020,24 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
-      <c r="H72" s="2" t="s">
+      <c r="H72" s="2"/>
+      <c r="I72" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I72" s="2" t="s">
+      <c r="J72" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="J72">
+      <c r="K72">
         <v>173</v>
-      </c>
-      <c r="K72" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="L72" s="2" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="73" spans="1:14">
+      <c r="M72" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -3879,23 +4045,24 @@
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
-      <c r="H73" s="2" t="s">
+      <c r="H73" s="2"/>
+      <c r="I73" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I73" s="2" t="s">
+      <c r="J73" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="J73">
+      <c r="K73">
         <v>173</v>
-      </c>
-      <c r="K73" s="2" t="s">
-        <v>297</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="74" spans="1:14">
+      <c r="M73" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -3903,21 +4070,22 @@
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
-      <c r="H74" s="2" t="s">
+      <c r="H74" s="2"/>
+      <c r="I74" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I74" s="2" t="s">
+      <c r="J74" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="J74">
+      <c r="K74">
         <v>5</v>
       </c>
-      <c r="K74" s="2" t="s">
+      <c r="L74" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="L74" s="2"/>
-    </row>
-    <row r="75" spans="1:14">
+      <c r="M74" s="2"/>
+    </row>
+    <row r="75" spans="1:15">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -3925,21 +4093,22 @@
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
-      <c r="H75" s="2" t="s">
+      <c r="H75" s="2"/>
+      <c r="I75" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I75" s="2" t="s">
+      <c r="J75" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="J75">
+      <c r="K75">
         <v>5</v>
       </c>
-      <c r="K75" s="2" t="s">
+      <c r="L75" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="L75" s="2"/>
-    </row>
-    <row r="76" spans="1:14">
+      <c r="M75" s="2"/>
+    </row>
+    <row r="76" spans="1:15">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -3947,24 +4116,25 @@
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
-      <c r="H76" s="2" t="s">
+      <c r="H76" s="2"/>
+      <c r="I76" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I76" s="2" t="s">
+      <c r="J76" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="J76">
+      <c r="K76">
         <v>5</v>
       </c>
-      <c r="K76" s="2" t="s">
+      <c r="L76" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="L76" s="2"/>
-      <c r="M76" t="s">
+      <c r="M76" s="2"/>
+      <c r="N76" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="77" spans="1:14">
+    <row r="77" spans="1:15">
       <c r="A77" s="2" t="s">
         <v>55</v>
       </c>
@@ -3983,49 +4153,54 @@
       <c r="F77" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="G77" s="2"/>
-      <c r="H77" s="2" t="s">
+      <c r="G77" s="2" t="s">
         <v>139</v>
       </c>
+      <c r="H77" s="6" t="b">
+        <f>EXACT(F77,G77)</f>
+        <v>1</v>
+      </c>
       <c r="I77" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J77" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="J77"/>
-      <c r="K77" s="2" t="s">
-        <v>225</v>
-      </c>
+      <c r="K77"/>
       <c r="L77" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="N77" t="s">
+      <c r="M77" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="O77" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="78" spans="1:14">
+    <row r="78" spans="1:15">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
-      <c r="G78" s="2" t="s">
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H78" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="I78" s="2" t="s">
+      <c r="J78" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="J78"/>
-      <c r="K78" s="2" t="s">
-        <v>195</v>
-      </c>
+      <c r="K78"/>
       <c r="L78" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="79" spans="1:14">
+      <c r="M78" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -4033,21 +4208,22 @@
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
-      <c r="H79" s="2" t="s">
+      <c r="H79" s="2"/>
+      <c r="I79" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I79" s="2" t="s">
+      <c r="J79" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="J79">
+      <c r="K79">
         <v>187</v>
       </c>
-      <c r="K79" s="2" t="s">
+      <c r="L79" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="L79" s="2"/>
-    </row>
-    <row r="80" spans="1:14">
+      <c r="M79" s="2"/>
+    </row>
+    <row r="80" spans="1:15">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -4055,21 +4231,22 @@
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
-      <c r="H80" s="2" t="s">
+      <c r="H80" s="2"/>
+      <c r="I80" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I80" s="2" t="s">
+      <c r="J80" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="J80">
+      <c r="K80">
         <v>187</v>
       </c>
-      <c r="K80" s="2" t="s">
+      <c r="L80" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="L80" s="2"/>
-    </row>
-    <row r="81" spans="1:14">
+      <c r="M80" s="2"/>
+    </row>
+    <row r="81" spans="1:15">
       <c r="A81" s="2" t="s">
         <v>56</v>
       </c>
@@ -4088,51 +4265,56 @@
       <c r="F81" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G81" s="2"/>
-      <c r="H81" s="2" t="s">
+      <c r="G81" s="2" t="s">
         <v>137</v>
       </c>
+      <c r="H81" s="6" t="b">
+        <f>EXACT(F81,G81)</f>
+        <v>1</v>
+      </c>
       <c r="I81" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J81" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="J81">
+      <c r="K81">
         <v>2035</v>
-      </c>
-      <c r="K81" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="L81" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="N81" s="2" t="s">
+      <c r="M81" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="O81" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="82" spans="1:14">
+    <row r="82" spans="1:15">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
-      <c r="G82" s="2" t="s">
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="H82" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="I82" s="2" t="s">
+      <c r="J82" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="J82">
+      <c r="K82">
         <v>2035</v>
       </c>
-      <c r="K82" s="2" t="s">
+      <c r="L82" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="L82" s="2"/>
-    </row>
-    <row r="83" spans="1:14">
+      <c r="M82" s="2"/>
+    </row>
+    <row r="83" spans="1:15">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -4140,21 +4322,22 @@
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
-      <c r="H83" s="2" t="s">
+      <c r="H83" s="2"/>
+      <c r="I83" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I83" s="2" t="s">
+      <c r="J83" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="J83">
+      <c r="K83">
         <v>2035</v>
       </c>
-      <c r="K83" s="2" t="s">
+      <c r="L83" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="L83" s="2"/>
-    </row>
-    <row r="84" spans="1:14">
+      <c r="M83" s="2"/>
+    </row>
+    <row r="84" spans="1:15">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -4162,21 +4345,22 @@
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
-      <c r="H84" s="2" t="s">
+      <c r="H84" s="2"/>
+      <c r="I84" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I84" s="2" t="s">
+      <c r="J84" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="J84">
+      <c r="K84">
         <v>2035</v>
       </c>
-      <c r="K84" s="2" t="s">
+      <c r="L84" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="L84" s="2"/>
-    </row>
-    <row r="85" spans="1:14">
+      <c r="M84" s="2"/>
+    </row>
+    <row r="85" spans="1:15">
       <c r="A85" s="2" t="s">
         <v>59</v>
       </c>
@@ -4195,51 +4379,56 @@
       <c r="F85" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2" t="s">
+      <c r="G85" s="2" t="s">
         <v>137</v>
       </c>
+      <c r="H85" s="6" t="b">
+        <f>EXACT(F85,G85)</f>
+        <v>0</v>
+      </c>
       <c r="I85" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J85" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="J85">
+      <c r="K85">
         <v>451</v>
-      </c>
-      <c r="K85" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="L85" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="N85" s="2" t="s">
+      <c r="M85" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="O85" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="86" spans="1:14">
+    <row r="86" spans="1:15">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
-      <c r="G86" s="2" t="s">
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="H86" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="I86" s="2" t="s">
+      <c r="J86" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="J86">
+      <c r="K86">
         <v>450</v>
       </c>
-      <c r="K86" s="2" t="s">
+      <c r="L86" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="L86" s="2"/>
-    </row>
-    <row r="87" spans="1:14">
+      <c r="M86" s="2"/>
+    </row>
+    <row r="87" spans="1:15">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -4247,23 +4436,24 @@
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
-      <c r="H87" s="2" t="s">
+      <c r="H87" s="2"/>
+      <c r="I87" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I87" s="8" t="s">
+      <c r="J87" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="J87">
+      <c r="K87">
         <v>447</v>
-      </c>
-      <c r="K87" t="s">
-        <v>183</v>
       </c>
       <c r="L87" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="88" spans="1:14">
+      <c r="M87" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -4271,21 +4461,22 @@
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
-      <c r="H88" s="2" t="s">
+      <c r="H88" s="2"/>
+      <c r="I88" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I88" s="8" t="s">
+      <c r="J88" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="J88">
+      <c r="K88">
         <v>448</v>
       </c>
-      <c r="K88" s="2" t="s">
+      <c r="L88" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="L88" s="2"/>
-    </row>
-    <row r="89" spans="1:14">
+      <c r="M88" s="2"/>
+    </row>
+    <row r="89" spans="1:15">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -4293,23 +4484,24 @@
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
-      <c r="H89" s="2" t="s">
+      <c r="H89" s="2"/>
+      <c r="I89" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I89" s="8" t="s">
+      <c r="J89" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="J89">
+      <c r="K89">
         <v>448</v>
-      </c>
-      <c r="K89" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="L89" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="90" spans="1:14">
+      <c r="M89" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -4317,23 +4509,24 @@
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
-      <c r="H90" s="2" t="s">
+      <c r="H90" s="2"/>
+      <c r="I90" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I90" s="8" t="s">
+      <c r="J90" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="J90">
+      <c r="K90">
         <v>448</v>
-      </c>
-      <c r="K90" s="2" t="s">
-        <v>296</v>
       </c>
       <c r="L90" s="2" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="91" spans="1:14">
+      <c r="M90" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -4341,23 +4534,24 @@
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
-      <c r="H91" s="2" t="s">
+      <c r="H91" s="2"/>
+      <c r="I91" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="I91" s="8" t="s">
+      <c r="J91" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="J91">
+      <c r="K91">
         <v>450</v>
-      </c>
-      <c r="K91" s="2" t="s">
-        <v>285</v>
       </c>
       <c r="L91" s="2" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="92" spans="1:14">
+      <c r="M91" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15">
       <c r="A92" s="2" t="s">
         <v>61</v>
       </c>
@@ -4376,27 +4570,33 @@
       <c r="F92" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G92" s="2"/>
-      <c r="H92" s="2" t="s">
+      <c r="G92" s="2" t="s">
         <v>137</v>
       </c>
+      <c r="H92" s="6" t="b">
+        <f>EXACT(F92,G92)</f>
+        <v>1</v>
+      </c>
       <c r="I92" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J92" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="J92">
+      <c r="K92">
         <v>984</v>
-      </c>
-      <c r="K92" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="N92" t="s">
+      <c r="M92" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="O92" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="93" spans="1:14">
+    <row r="93" spans="1:15">
       <c r="A93" s="2" t="s">
         <v>64</v>
       </c>
@@ -4416,50 +4616,53 @@
         <v>138</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="H93" s="2" t="s">
         <v>142</v>
       </c>
+      <c r="H93" s="6" t="b">
+        <f>EXACT(F93,G93)</f>
+        <v>0</v>
+      </c>
       <c r="I93" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J93" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="J93"/>
-      <c r="K93" s="2" t="s">
-        <v>296</v>
-      </c>
+      <c r="K93"/>
       <c r="L93" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="N93" s="2" t="s">
+      <c r="M93" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="O93" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="94" spans="1:14">
+    <row r="94" spans="1:15">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
-      <c r="G94" s="2" t="s">
+      <c r="G94" s="2"/>
+      <c r="H94" s="2"/>
+      <c r="I94" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="H94" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="I94" s="2" t="s">
+      <c r="J94" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="J94"/>
-      <c r="K94" s="2" t="s">
-        <v>159</v>
-      </c>
+      <c r="K94"/>
       <c r="L94" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="95" spans="1:14">
+      <c r="M94" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -4467,21 +4670,22 @@
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
-      <c r="H95" s="2" t="s">
+      <c r="H95" s="2"/>
+      <c r="I95" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I95" s="2" t="s">
+      <c r="J95" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="J95"/>
-      <c r="K95" s="2" t="s">
-        <v>153</v>
-      </c>
+      <c r="K95"/>
       <c r="L95" s="2" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="96" spans="1:14">
+      <c r="M95" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -4489,21 +4693,22 @@
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
-      <c r="H96" s="2" t="s">
+      <c r="H96" s="2"/>
+      <c r="I96" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I96" s="2" t="s">
+      <c r="J96" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="J96"/>
-      <c r="K96" s="2" t="s">
-        <v>191</v>
-      </c>
+      <c r="K96"/>
       <c r="L96" s="2" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="97" spans="1:14">
+      <c r="M96" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15">
       <c r="A97" s="2" t="s">
         <v>66</v>
       </c>
@@ -4522,43 +4727,55 @@
       <c r="F97" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G97" s="2"/>
-      <c r="H97" s="2" t="s">
+      <c r="G97" t="s">
         <v>137</v>
       </c>
-      <c r="I97" s="8" t="s">
+      <c r="H97" s="6" t="b">
+        <f>EXACT(F97,G97)</f>
+        <v>1</v>
+      </c>
+      <c r="I97" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J97" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="J97">
+      <c r="K97">
         <v>318</v>
-      </c>
-      <c r="K97" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="L97" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="N97" t="s">
+      <c r="M97" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="O97" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="98" spans="1:14">
-      <c r="G98" t="s">
+    <row r="98" spans="1:15">
+      <c r="I98" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="H98" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="I98" s="2" t="s">
+      <c r="J98" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="J98"/>
-      <c r="K98" s="2" t="s">
+      <c r="K98"/>
+      <c r="L98" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="L98" s="2"/>
-    </row>
-    <row r="103" spans="1:14">
+      <c r="M98" s="2"/>
+    </row>
+    <row r="102" spans="1:15">
+      <c r="G102" t="s">
+        <v>303</v>
+      </c>
+      <c r="H102">
+        <f>COUNTA(H2:H101)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15">
       <c r="A103" t="s">
         <v>137</v>
       </c>
@@ -4570,11 +4787,18 @@
         <v>225</v>
       </c>
       <c r="E103">
-        <f>COUNTIF(L:L, D103)</f>
+        <f t="shared" ref="E103:E116" si="0">COUNTIF(M:M, D103)</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="104" spans="1:14">
+      <c r="G103" t="s">
+        <v>304</v>
+      </c>
+      <c r="H103">
+        <f>COUNTIF(H2:H101,TRUE)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15">
       <c r="A104" t="s">
         <v>142</v>
       </c>
@@ -4586,66 +4810,80 @@
         <v>153</v>
       </c>
       <c r="E104">
-        <f>COUNTIF(L:L, D104)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="105" spans="1:14">
+      <c r="G104" t="s">
+        <v>305</v>
+      </c>
+      <c r="H104">
+        <f>H102-H103</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15">
       <c r="A105" t="s">
         <v>140</v>
       </c>
       <c r="B105">
-        <f t="shared" ref="B105:B107" si="0">COUNTIF(G:G, A105)</f>
+        <f t="shared" ref="B105:B107" si="1">COUNTIF(G:G, A105)</f>
         <v>3</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>166</v>
       </c>
       <c r="E105">
-        <f>COUNTIF(L:L, D105)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="M105" t="s">
+      <c r="G105" t="s">
+        <v>306</v>
+      </c>
+      <c r="H105">
+        <f>H103/H102</f>
+        <v>0.64</v>
+      </c>
+      <c r="N105" t="s">
         <v>230</v>
       </c>
-      <c r="N105">
-        <f>COUNTIF(N2:N97, "Ja")</f>
+      <c r="O105">
+        <f>COUNTIF(O2:O97, "Ja")</f>
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:14">
+    <row r="106" spans="1:15">
       <c r="A106" t="s">
         <v>141</v>
       </c>
       <c r="B106">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>159</v>
       </c>
       <c r="E106">
-        <f>COUNTIF(L:L, D106)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:14">
+    <row r="107" spans="1:15">
       <c r="A107" t="s">
         <v>139</v>
       </c>
       <c r="B107">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>182</v>
       </c>
       <c r="E107">
-        <f>COUNTIF(L:L, D107)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:14">
+    <row r="108" spans="1:15">
       <c r="B108">
         <f>SUM(B103:B107)</f>
         <v>25</v>
@@ -4654,43 +4892,43 @@
         <v>171</v>
       </c>
       <c r="E108">
-        <f>COUNTIF(L:L, D108)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:14">
+    <row r="109" spans="1:15">
       <c r="D109" s="2" t="s">
         <v>191</v>
       </c>
       <c r="E109">
-        <f>COUNTIF(L:L, D109)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:14">
+    <row r="110" spans="1:15">
       <c r="D110" s="2" t="s">
         <v>174</v>
       </c>
       <c r="E110">
-        <f>COUNTIF(L:L, D110)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:14">
+    <row r="111" spans="1:15">
       <c r="D111" s="2" t="s">
         <v>295</v>
       </c>
       <c r="E111">
-        <f>COUNTIF(L:L, D111)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:14">
+    <row r="112" spans="1:15">
       <c r="D112" t="s">
         <v>183</v>
       </c>
       <c r="E112">
-        <f>COUNTIF(L:L, D112)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -4699,7 +4937,7 @@
         <v>186</v>
       </c>
       <c r="E113">
-        <f>COUNTIF(L:L, D113)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -4708,7 +4946,7 @@
         <v>294</v>
       </c>
       <c r="E114">
-        <f>COUNTIF(L:L, D114)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -4717,7 +4955,7 @@
         <v>297</v>
       </c>
       <c r="E115">
-        <f>COUNTIF(L:L, D115)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -4726,7 +4964,7 @@
         <v>296</v>
       </c>
       <c r="E116">
-        <f>COUNTIF(L:L, D116)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -7773,7 +8011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
@@ -7959,23 +8197,23 @@
         <v>159</v>
       </c>
       <c r="C3" s="30">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B3,Gefiltert!$H:$H,C$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B3,Gefiltert!$I:$I,C$1)</f>
         <v>1</v>
       </c>
       <c r="D3">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B3,Gefiltert!$H:$H,D$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B3,Gefiltert!$I:$I,D$1)</f>
         <v>4</v>
       </c>
       <c r="E3">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B3,Gefiltert!$H:$H,E$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B3,Gefiltert!$I:$I,E$1)</f>
         <v>1</v>
       </c>
       <c r="F3">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B3,Gefiltert!$H:$H,F$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B3,Gefiltert!$I:$I,F$1)</f>
         <v>2</v>
       </c>
       <c r="G3">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B3,Gefiltert!$H:$H,G$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B3,Gefiltert!$I:$I,G$1)</f>
         <v>7</v>
       </c>
       <c r="H3" s="30">
@@ -7988,23 +8226,23 @@
         <v>182</v>
       </c>
       <c r="C4" s="30">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B4,Gefiltert!$H:$H,C$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B4,Gefiltert!$I:$I,C$1)</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B4,Gefiltert!$H:$H,D$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B4,Gefiltert!$I:$I,D$1)</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B4,Gefiltert!$H:$H,E$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B4,Gefiltert!$I:$I,E$1)</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B4,Gefiltert!$H:$H,F$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B4,Gefiltert!$I:$I,F$1)</f>
         <v>1</v>
       </c>
       <c r="G4">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B4,Gefiltert!$H:$H,G$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B4,Gefiltert!$I:$I,G$1)</f>
         <v>2</v>
       </c>
       <c r="H4" s="30">
@@ -8017,23 +8255,23 @@
         <v>295</v>
       </c>
       <c r="C5" s="30">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B5,Gefiltert!$H:$H,C$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B5,Gefiltert!$I:$I,C$1)</f>
         <v>0</v>
       </c>
       <c r="D5">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B5,Gefiltert!$H:$H,D$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B5,Gefiltert!$I:$I,D$1)</f>
         <v>0</v>
       </c>
       <c r="E5">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B5,Gefiltert!$H:$H,E$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B5,Gefiltert!$I:$I,E$1)</f>
         <v>1</v>
       </c>
       <c r="F5">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B5,Gefiltert!$H:$H,F$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B5,Gefiltert!$I:$I,F$1)</f>
         <v>0</v>
       </c>
       <c r="G5">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B5,Gefiltert!$H:$H,G$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B5,Gefiltert!$I:$I,G$1)</f>
         <v>2</v>
       </c>
       <c r="H5" s="30">
@@ -8046,23 +8284,23 @@
         <v>296</v>
       </c>
       <c r="C6" s="29">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B6,Gefiltert!$H:$H,C$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B6,Gefiltert!$I:$I,C$1)</f>
         <v>1</v>
       </c>
       <c r="D6" s="26">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B6,Gefiltert!$H:$H,D$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B6,Gefiltert!$I:$I,D$1)</f>
         <v>2</v>
       </c>
       <c r="E6" s="26">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B6,Gefiltert!$H:$H,E$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B6,Gefiltert!$I:$I,E$1)</f>
         <v>1</v>
       </c>
       <c r="F6" s="26">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B6,Gefiltert!$H:$H,F$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B6,Gefiltert!$I:$I,F$1)</f>
         <v>0</v>
       </c>
       <c r="G6" s="26">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B6,Gefiltert!$H:$H,G$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B6,Gefiltert!$I:$I,G$1)</f>
         <v>1</v>
       </c>
       <c r="H6" s="29">
@@ -8110,23 +8348,23 @@
         <v>166</v>
       </c>
       <c r="C9" s="30">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B9,Gefiltert!$H:$H,C$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B9,Gefiltert!$I:$I,C$1)</f>
         <v>0</v>
       </c>
       <c r="D9">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B9,Gefiltert!$H:$H,D$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B9,Gefiltert!$I:$I,D$1)</f>
         <v>0</v>
       </c>
       <c r="E9">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B9,Gefiltert!$H:$H,E$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B9,Gefiltert!$I:$I,E$1)</f>
         <v>0</v>
       </c>
       <c r="F9">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B9,Gefiltert!$H:$H,F$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B9,Gefiltert!$I:$I,F$1)</f>
         <v>1</v>
       </c>
       <c r="G9">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B9,Gefiltert!$H:$H,G$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B9,Gefiltert!$I:$I,G$1)</f>
         <v>2</v>
       </c>
       <c r="H9" s="30">
@@ -8139,23 +8377,23 @@
         <v>174</v>
       </c>
       <c r="C10" s="30">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B10,Gefiltert!$H:$H,C$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B10,Gefiltert!$I:$I,C$1)</f>
         <v>0</v>
       </c>
       <c r="D10">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B10,Gefiltert!$H:$H,D$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B10,Gefiltert!$I:$I,D$1)</f>
         <v>2</v>
       </c>
       <c r="E10">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B10,Gefiltert!$H:$H,E$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B10,Gefiltert!$I:$I,E$1)</f>
         <v>0</v>
       </c>
       <c r="F10">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B10,Gefiltert!$H:$H,F$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B10,Gefiltert!$I:$I,F$1)</f>
         <v>0</v>
       </c>
       <c r="G10">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B10,Gefiltert!$H:$H,G$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B10,Gefiltert!$I:$I,G$1)</f>
         <v>1</v>
       </c>
       <c r="H10" s="30">
@@ -8202,23 +8440,23 @@
         <v>171</v>
       </c>
       <c r="C13" s="30">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B13,Gefiltert!$H:$H,C$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B13,Gefiltert!$I:$I,C$1)</f>
         <v>1</v>
       </c>
       <c r="D13">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B13,Gefiltert!$H:$H,D$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B13,Gefiltert!$I:$I,D$1)</f>
         <v>0</v>
       </c>
       <c r="E13">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B13,Gefiltert!$H:$H,E$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B13,Gefiltert!$I:$I,E$1)</f>
         <v>0</v>
       </c>
       <c r="F13">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B13,Gefiltert!$H:$H,F$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B13,Gefiltert!$I:$I,F$1)</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B13,Gefiltert!$H:$H,G$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B13,Gefiltert!$I:$I,G$1)</f>
         <v>0</v>
       </c>
       <c r="H13" s="30">
@@ -8231,23 +8469,23 @@
         <v>183</v>
       </c>
       <c r="C14" s="30">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B14,Gefiltert!$H:$H,C$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B14,Gefiltert!$I:$I,C$1)</f>
         <v>1</v>
       </c>
       <c r="D14">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B14,Gefiltert!$H:$H,D$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B14,Gefiltert!$I:$I,D$1)</f>
         <v>0</v>
       </c>
       <c r="E14">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B14,Gefiltert!$H:$H,E$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B14,Gefiltert!$I:$I,E$1)</f>
         <v>1</v>
       </c>
       <c r="F14">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B14,Gefiltert!$H:$H,F$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B14,Gefiltert!$I:$I,F$1)</f>
         <v>0</v>
       </c>
       <c r="G14">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B14,Gefiltert!$H:$H,G$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B14,Gefiltert!$I:$I,G$1)</f>
         <v>0</v>
       </c>
       <c r="H14" s="30">
@@ -8260,23 +8498,23 @@
         <v>294</v>
       </c>
       <c r="C15" s="30">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B15,Gefiltert!$H:$H,C$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B15,Gefiltert!$I:$I,C$1)</f>
         <v>0</v>
       </c>
       <c r="D15">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B15,Gefiltert!$H:$H,D$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B15,Gefiltert!$I:$I,D$1)</f>
         <v>0</v>
       </c>
       <c r="E15">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B15,Gefiltert!$H:$H,E$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B15,Gefiltert!$I:$I,E$1)</f>
         <v>0</v>
       </c>
       <c r="F15">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B15,Gefiltert!$H:$H,F$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B15,Gefiltert!$I:$I,F$1)</f>
         <v>1</v>
       </c>
       <c r="G15">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B15,Gefiltert!$H:$H,G$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B15,Gefiltert!$I:$I,G$1)</f>
         <v>1</v>
       </c>
       <c r="H15" s="30">
@@ -8323,23 +8561,23 @@
         <v>154</v>
       </c>
       <c r="C18" s="30">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B18,Gefiltert!$H:$H,C$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B18,Gefiltert!$I:$I,C$1)</f>
         <v>6</v>
       </c>
       <c r="D18">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B18,Gefiltert!$H:$H,D$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B18,Gefiltert!$I:$I,D$1)</f>
         <v>4</v>
       </c>
       <c r="E18">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B18,Gefiltert!$H:$H,E$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B18,Gefiltert!$I:$I,E$1)</f>
         <v>1</v>
       </c>
       <c r="F18">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B18,Gefiltert!$H:$H,F$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B18,Gefiltert!$I:$I,F$1)</f>
         <v>1</v>
       </c>
       <c r="G18">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B18,Gefiltert!$H:$H,G$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B18,Gefiltert!$I:$I,G$1)</f>
         <v>6</v>
       </c>
       <c r="H18" s="30">
@@ -8352,23 +8590,23 @@
         <v>297</v>
       </c>
       <c r="C19" s="30">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B19,Gefiltert!$H:$H,C$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B19,Gefiltert!$I:$I,C$1)</f>
         <v>0</v>
       </c>
       <c r="D19">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B19,Gefiltert!$H:$H,D$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B19,Gefiltert!$I:$I,D$1)</f>
         <v>0</v>
       </c>
       <c r="E19">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B19,Gefiltert!$H:$H,E$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B19,Gefiltert!$I:$I,E$1)</f>
         <v>0</v>
       </c>
       <c r="F19">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B19,Gefiltert!$H:$H,F$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B19,Gefiltert!$I:$I,F$1)</f>
         <v>1</v>
       </c>
       <c r="G19">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B19,Gefiltert!$H:$H,G$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B19,Gefiltert!$I:$I,G$1)</f>
         <v>2</v>
       </c>
       <c r="H19" s="30">
@@ -8415,23 +8653,23 @@
         <v>153</v>
       </c>
       <c r="C22" s="30">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B22,Gefiltert!$H:$H,C$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B22,Gefiltert!$I:$I,C$1)</f>
         <v>1</v>
       </c>
       <c r="D22">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B22,Gefiltert!$H:$H,D$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B22,Gefiltert!$I:$I,D$1)</f>
         <v>1</v>
       </c>
       <c r="E22">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B22,Gefiltert!$H:$H,E$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B22,Gefiltert!$I:$I,E$1)</f>
         <v>0</v>
       </c>
       <c r="F22">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B22,Gefiltert!$H:$H,F$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B22,Gefiltert!$I:$I,F$1)</f>
         <v>0</v>
       </c>
       <c r="G22">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B22,Gefiltert!$H:$H,G$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B22,Gefiltert!$I:$I,G$1)</f>
         <v>0</v>
       </c>
       <c r="H22" s="30">
@@ -8478,23 +8716,23 @@
         <v>300</v>
       </c>
       <c r="C25" s="30">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B25,Gefiltert!$H:$H,C$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B25,Gefiltert!$I:$I,C$1)</f>
         <v>1</v>
       </c>
       <c r="D25">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B25,Gefiltert!$H:$H,D$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B25,Gefiltert!$I:$I,D$1)</f>
         <v>2</v>
       </c>
       <c r="E25">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B25,Gefiltert!$H:$H,E$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B25,Gefiltert!$I:$I,E$1)</f>
         <v>0</v>
       </c>
       <c r="F25">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B25,Gefiltert!$H:$H,F$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B25,Gefiltert!$I:$I,F$1)</f>
         <v>1</v>
       </c>
       <c r="G25">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B25,Gefiltert!$H:$H,G$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B25,Gefiltert!$I:$I,G$1)</f>
         <v>0</v>
       </c>
       <c r="H25" s="30">
@@ -8507,23 +8745,23 @@
         <v>285</v>
       </c>
       <c r="C26" s="30">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B26,Gefiltert!$H:$H,C$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B26,Gefiltert!$I:$I,C$1)</f>
         <v>2</v>
       </c>
       <c r="D26">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B26,Gefiltert!$H:$H,D$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B26,Gefiltert!$I:$I,D$1)</f>
         <v>0</v>
       </c>
       <c r="E26">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B26,Gefiltert!$H:$H,E$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B26,Gefiltert!$I:$I,E$1)</f>
         <v>0</v>
       </c>
       <c r="F26">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B26,Gefiltert!$H:$H,F$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B26,Gefiltert!$I:$I,F$1)</f>
         <v>0</v>
       </c>
       <c r="G26">
-        <f>COUNTIFS(Gefiltert!$L:$L,$B26,Gefiltert!$H:$H,G$1)</f>
+        <f>COUNTIFS(Gefiltert!$M:$M,$B26,Gefiltert!$I:$I,G$1)</f>
         <v>1</v>
       </c>
       <c r="H26" s="30">

</xml_diff>

<commit_message>
Zwischenspeichern. Mehr Kennzahlen für Mapping (Prozente etc.)
</commit_message>
<xml_diff>
--- a/Review.xlsx
+++ b/Review.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24709"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16080" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Gefiltert" sheetId="2" r:id="rId1"/>
@@ -1026,7 +1026,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1085,6 +1085,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1218,7 +1225,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="139">
+  <cellStyleXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1358,8 +1365,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1420,8 +1434,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="139" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="139">
+  <cellStyles count="146">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -1491,6 +1506,9 @@
     <cellStyle name="Besuchter Link" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="145" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1560,6 +1578,10 @@
     <cellStyle name="Link" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Prozent" xfId="139" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1835,7 +1857,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1845,9 +1867,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G102" sqref="G102:H105"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J106" sqref="J106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4783,6 +4805,10 @@
         <f>COUNTIF(G:G, A103)</f>
         <v>7</v>
       </c>
+      <c r="C103" s="38">
+        <f>B103/$B$108</f>
+        <v>0.28000000000000003</v>
+      </c>
       <c r="D103" t="s">
         <v>225</v>
       </c>
@@ -4806,6 +4832,10 @@
         <f>COUNTIF(G:G, A104)</f>
         <v>5</v>
       </c>
+      <c r="C104" s="38">
+        <f t="shared" ref="C104:C107" si="1">B104/$B$108</f>
+        <v>0.2</v>
+      </c>
       <c r="D104" t="s">
         <v>153</v>
       </c>
@@ -4826,8 +4856,12 @@
         <v>140</v>
       </c>
       <c r="B105">
-        <f t="shared" ref="B105:B107" si="1">COUNTIF(G:G, A105)</f>
+        <f t="shared" ref="B105:B107" si="2">COUNTIF(G:G, A105)</f>
         <v>3</v>
+      </c>
+      <c r="C105" s="38">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>166</v>
@@ -4856,8 +4890,12 @@
         <v>141</v>
       </c>
       <c r="B106">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="C106" s="38">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0.08</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>159</v>
@@ -4872,8 +4910,12 @@
         <v>139</v>
       </c>
       <c r="B107">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="C107" s="38">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>0.32</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>182</v>
@@ -8151,10 +8193,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8795,6 +8837,58 @@
         <v>7</v>
       </c>
     </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <f>COUNTA(A2:A28)</f>
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <f>COUNTA(B2:B28)</f>
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <f>COUNTIF(C2:C27,"&gt;0")-$A$29</f>
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ref="D29:G29" si="1">COUNTIF(D2:D27,"&gt;0")-$A$29</f>
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="C30" s="38">
+        <f>C29/$B$29</f>
+        <v>0.5</v>
+      </c>
+      <c r="D30" s="38">
+        <f t="shared" ref="D30:G30" si="2">D29/$B$29</f>
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="E30" s="38">
+        <f t="shared" si="2"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="F30" s="38">
+        <f t="shared" si="2"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="G30" s="38">
+        <f t="shared" si="2"/>
+        <v>0.6428571428571429</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>